<commit_message>
Hid columns C an D, which were for ACS 2012-2016, no longer needed.
</commit_message>
<xml_diff>
--- a/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
+++ b/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
@@ -1,32 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\petrale\applications\travel_model_lu_inputs\2015\Workers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\taz-data-baseyears\2015\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D17AEC2-CF86-4739-9744-4C6721B0D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13575" activeTab="1"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Workers" sheetId="1" r:id="rId1"/>
     <sheet name="Households by No. of Workers" sheetId="2" r:id="rId2"/>
     <sheet name="HHs by Workers Correction Fact." sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shimon Israel</author>
   </authors>
   <commentList>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,12 +70,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shimon Israel</author>
   </authors>
   <commentList>
-    <comment ref="P7" authorId="0" shapeId="0">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0">
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0">
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -368,7 +382,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
@@ -1055,7 +1069,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,14 +1091,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1095,14 +1109,18 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1117,12 +1135,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1444,59 +1456,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.08203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.58203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="31.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="33" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1555,7 @@
         <v>3.4305029999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>536209</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1597,7 @@
         <v>130747</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1618,7 @@
         <v>71146</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1627,7 +1639,7 @@
         <v>505329</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1648,7 +1660,7 @@
         <v>405183</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>967863</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1690,7 +1702,7 @@
         <v>200569</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1711,7 +1723,7 @@
         <v>250010</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1747,54 +1759,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.58203125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.58203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.75" style="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="31.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.08203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.75" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="33" t="s">
@@ -1821,7 +1833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1852,17 +1864,17 @@
       <c r="J6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="32" t="s">
         <v>30</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1922,7 @@
         <f>K7/E7</f>
         <v>0.61093155138835786</v>
       </c>
-      <c r="N7" s="32"/>
+      <c r="N7" s="15"/>
       <c r="O7" s="16" t="s">
         <v>31</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>3.4305029999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1962,9 +1974,9 @@
         <f t="shared" ref="M8:M56" si="0">K8/E8</f>
         <v>1.0636388531450143</v>
       </c>
-      <c r="N8" s="32"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2008,9 +2020,9 @@
         <f t="shared" si="0"/>
         <v>1.1506869686500032</v>
       </c>
-      <c r="N9" s="32"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
         <v>9</v>
@@ -2055,9 +2067,9 @@
         <f t="shared" si="0"/>
         <v>1.3420147906012951</v>
       </c>
-      <c r="N10" s="32"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -2104,9 +2116,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N11" s="32"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2154,9 +2166,9 @@
         <f>K12/E12</f>
         <v>0.81432449606111224</v>
       </c>
-      <c r="N12" s="32"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2200,9 +2212,9 @@
         <f t="shared" si="0"/>
         <v>1.0207878838846087</v>
       </c>
-      <c r="N13" s="32"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2246,9 +2258,9 @@
         <f t="shared" si="0"/>
         <v>1.0761103527203895</v>
       </c>
-      <c r="N14" s="32"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>9</v>
@@ -2293,9 +2305,9 @@
         <f t="shared" si="0"/>
         <v>1.1536676698765049</v>
       </c>
-      <c r="N15" s="32"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2342,9 +2354,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N16" s="32"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2392,9 +2404,9 @@
         <f>K17/E17</f>
         <v>0.81952491588983412</v>
       </c>
-      <c r="N17" s="32"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
@@ -2438,9 +2450,9 @@
         <f t="shared" si="0"/>
         <v>1.0466453858424083</v>
       </c>
-      <c r="N18" s="32"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
@@ -2484,9 +2496,9 @@
         <f t="shared" si="0"/>
         <v>1.0649963701049894</v>
       </c>
-      <c r="N19" s="32"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>9</v>
@@ -2531,9 +2543,9 @@
         <f t="shared" si="0"/>
         <v>1.1826070606325927</v>
       </c>
-      <c r="N20" s="32"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -2580,10 +2592,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N21" s="32"/>
+      <c r="N21" s="15"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2631,9 +2643,9 @@
         <f>K22/E22</f>
         <v>0.71025600208376349</v>
       </c>
-      <c r="N22" s="32"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
@@ -2677,9 +2689,9 @@
         <f t="shared" si="0"/>
         <v>1.0667906227589079</v>
       </c>
-      <c r="N23" s="32"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
@@ -2723,9 +2735,9 @@
         <f t="shared" si="0"/>
         <v>1.0848258755408788</v>
       </c>
-      <c r="N24" s="32"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="12" t="s">
         <v>9</v>
@@ -2770,9 +2782,9 @@
         <f t="shared" si="0"/>
         <v>1.2652338137782535</v>
       </c>
-      <c r="N25" s="32"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2819,9 +2831,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N26" s="32"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -2869,9 +2881,9 @@
         <f>K27/E27</f>
         <v>0.7243926284066956</v>
       </c>
-      <c r="N27" s="32"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N27" s="15"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
@@ -2915,9 +2927,9 @@
         <f t="shared" si="0"/>
         <v>1.0549854708758115</v>
       </c>
-      <c r="N28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
@@ -2961,9 +2973,9 @@
         <f t="shared" si="0"/>
         <v>1.077399993791341</v>
       </c>
-      <c r="N29" s="32"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N29" s="15"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="12" t="s">
         <v>9</v>
@@ -3008,9 +3020,9 @@
         <f t="shared" si="0"/>
         <v>1.2175676189166291</v>
       </c>
-      <c r="N30" s="32"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -3057,9 +3069,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3107,9 +3119,9 @@
         <f>K32/E32</f>
         <v>0.71045461057797943</v>
       </c>
-      <c r="N32" s="32"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
@@ -3153,9 +3165,9 @@
         <f t="shared" si="0"/>
         <v>1.0162564381618149</v>
       </c>
-      <c r="N33" s="32"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N33" s="15"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
@@ -3199,9 +3211,9 @@
         <f t="shared" si="0"/>
         <v>1.080655652908822</v>
       </c>
-      <c r="N34" s="32"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N34" s="15"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="12" t="s">
         <v>9</v>
@@ -3246,9 +3258,9 @@
         <f t="shared" si="0"/>
         <v>1.2111886446550346</v>
       </c>
-      <c r="N35" s="32"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N35" s="15"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
@@ -3295,9 +3307,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N36" s="32"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N36" s="15"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -3345,9 +3357,9 @@
         <f>K37/E37</f>
         <v>0.65234440973873298</v>
       </c>
-      <c r="N37" s="32"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N37" s="15"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
@@ -3391,9 +3403,9 @@
         <f t="shared" si="0"/>
         <v>1.0467479421237909</v>
       </c>
-      <c r="N38" s="32"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N38" s="15"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3437,9 +3449,9 @@
         <f t="shared" si="0"/>
         <v>1.0807546811717326</v>
       </c>
-      <c r="N39" s="32"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N39" s="15"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="12"/>
       <c r="B40" s="12" t="s">
         <v>9</v>
@@ -3484,9 +3496,9 @@
         <f t="shared" si="0"/>
         <v>1.2047919789524975</v>
       </c>
-      <c r="N40" s="32"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N40" s="15"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>27</v>
       </c>
@@ -3533,9 +3545,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N41" s="32"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N41" s="15"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -3583,9 +3595,9 @@
         <f>K42/E42</f>
         <v>0.79221032005758307</v>
       </c>
-      <c r="N42" s="32"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N42" s="15"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
@@ -3629,9 +3641,9 @@
         <f t="shared" si="0"/>
         <v>1.0348733305007278</v>
       </c>
-      <c r="N43" s="32"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N43" s="15"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>10</v>
       </c>
@@ -3675,9 +3687,9 @@
         <f t="shared" si="0"/>
         <v>1.1032421402931711</v>
       </c>
-      <c r="N44" s="32"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N44" s="15"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="12"/>
       <c r="B45" s="12" t="s">
         <v>9</v>
@@ -3722,9 +3734,9 @@
         <f t="shared" si="0"/>
         <v>1.1188919031557478</v>
       </c>
-      <c r="N45" s="32"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N45" s="15"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>28</v>
       </c>
@@ -3771,9 +3783,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N46" s="32"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N46" s="15"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -3821,9 +3833,9 @@
         <f>K47/E47</f>
         <v>0.81645903954103427</v>
       </c>
-      <c r="N47" s="32"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N47" s="15"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
@@ -3867,9 +3879,9 @@
         <f t="shared" si="0"/>
         <v>1.0465230399958017</v>
       </c>
-      <c r="N48" s="32"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N48" s="15"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>10</v>
       </c>
@@ -3913,9 +3925,9 @@
         <f t="shared" si="0"/>
         <v>1.0691305300394971</v>
       </c>
-      <c r="N49" s="32"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N49" s="15"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="12"/>
       <c r="B50" s="12" t="s">
         <v>9</v>
@@ -3960,9 +3972,9 @@
         <f t="shared" si="0"/>
         <v>1.1597473621148717</v>
       </c>
-      <c r="N50" s="32"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N50" s="15"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>29</v>
       </c>
@@ -4009,9 +4021,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N51" s="32"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N51" s="15"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>19</v>
       </c>
@@ -4062,9 +4074,9 @@
         <f>K52/E52</f>
         <v>0.71267571243523475</v>
       </c>
-      <c r="N52" s="32"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N52" s="15"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>11</v>
       </c>
@@ -4112,9 +4124,9 @@
         <f t="shared" si="0"/>
         <v>1.0445240294195008</v>
       </c>
-      <c r="N53" s="32"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N53" s="15"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>10</v>
       </c>
@@ -4162,9 +4174,9 @@
         <f t="shared" si="0"/>
         <v>1.093851897536487</v>
       </c>
-      <c r="N54" s="32"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N54" s="15"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="12"/>
       <c r="B55" s="12" t="s">
         <v>9</v>
@@ -4213,9 +4225,9 @@
         <f t="shared" si="0"/>
         <v>1.2188285577583124</v>
       </c>
-      <c r="N55" s="32"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="N55" s="15"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>20</v>
       </c>
@@ -4263,7 +4275,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N56" s="32"/>
+      <c r="N56" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4280,14 +4292,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="14.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.25" style="1" bestFit="1" customWidth="1"/>
@@ -4295,518 +4307,518 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="1">
         <v>0.7243926284066956</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="1">
         <v>0.71045461057797943</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="1">
         <v>0.65234440973873298</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="29">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="1">
         <v>0.61093155138835786</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="1">
         <v>0.81432449606111224</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="1">
         <v>0.79221032005758307</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="1">
         <v>0.71025600208376349</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>0.81645903954103427</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="29" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="1">
         <v>0.81952491588983412</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="1">
         <v>1.0549854708758115</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="1">
         <v>1.0162564381618149</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="1">
         <v>1.0467479421237909</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="29">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="1">
         <v>1.0636388531450143</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="1">
         <v>5</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="1">
         <v>1.0207878838846087</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="1">
         <v>1.0348733305007278</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="29" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="1">
         <v>7</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="1">
         <v>1.0667906227589079</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="29" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="1">
         <v>8</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="1">
         <v>1.0465230399958017</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="1">
         <v>9</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="1">
         <v>1.0466453858424083</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="29" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="1">
         <v>1.077399993791341</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="1">
         <v>1.080655652908822</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="1">
         <v>1.0807546811717326</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="29">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
         <v>4</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="1">
         <v>1.1506869686500032</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="29" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="1">
         <v>1.0761103527203895</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="29" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="1">
         <v>6</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="1">
         <v>1.1032421402931711</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="29" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="1">
         <v>7</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="1">
         <v>1.0848258755408788</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="29" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="1">
         <v>8</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="1">
         <v>1.0691305300394971</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="1">
         <v>9</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="1">
         <v>1.0649963701049894</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="1">
         <v>1.2175676189166291</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="1">
         <v>1.2111886446550346</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="1">
         <v>3</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D31" s="1">
         <v>1.2047919789524975</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="29">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
         <v>4</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="1">
         <v>1.3420147906012951</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="29" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="1">
         <v>5</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D33" s="1">
         <v>1.1536676698765049</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="1">
         <v>6</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="1">
         <v>1.1188919031557478</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="29" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="1">
         <v>7</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="1">
         <v>1.2652338137782535</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="29" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="29">
+      <c r="B36" s="1">
         <v>8</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D36" s="1">
         <v>1.1597473621148717</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="29" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="1">
         <v>9</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D37" s="1">
@@ -4814,7 +4826,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D37">
     <sortCondition ref="C2:C37"/>
     <sortCondition ref="B2:B37"/>
   </sortState>

</xml_diff>

<commit_message>
Updated descriptions within spreadsheet
</commit_message>
<xml_diff>
--- a/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
+++ b/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\taz-data-baseyears\2015\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D17AEC2-CF86-4739-9744-4C6721B0D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E4187C-FA53-4A8D-AF3D-BC2D1836D2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <author>Shimon Israel</author>
   </authors>
   <commentList>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -120,11 +120,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Implied HHs come from back-calculating workers to households, using average 3+ workers value to the right. </t>
+Implied HHs come from back-calculating workers to households, using average 3+ workers value (calculated from PUMS 2013-2017) to the right. </t>
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -144,11 +144,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Worker distribution here comes from 2013-2017 PUMS, factored to exactly match ACS 2013-2017.</t>
+Worker distribution here comes from 2013-2017 PUMS, scaled so totals exactly match ACS 2013-2017.</t>
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -172,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -200,8 +200,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Shimon Israel</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3F0BA09A-35E5-495C-9F55-9905CB8C7B43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shimon Israel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These come from Column K in "Households by No. of Workers" tab and were used to correct/rescale households by workers in the TAZ data building script. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="62">
   <si>
     <t>Alameda</t>
   </si>
@@ -366,17 +400,73 @@
     <t>PUMS 2013-2017 HH Weights</t>
   </si>
   <si>
-    <t>PUMS 2013-2017 Commuters (ESR==1,4), Using HH Weights</t>
-  </si>
-  <si>
-    <t>PUMS 2013-2017 Workers (ESR==1,2,4,5), Using Person Weights</t>
-  </si>
-  <si>
-    <t>PUMS 2012-2016 Workers (ESR==1,2,4,5), Using HH Weights</t>
-  </si>
-  <si>
     <t>ACS 2013-2017
 Refactored Using Total Worker Table (B23025) and PUMS 2013-2017</t>
+  </si>
+  <si>
+    <r>
+      <t>PUMS 2013-2017 Commuters (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ESR==1,4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), Using HH Weights</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PUMS 2013-2017 Workers (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ESR==1,2,4,5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), Using Person Weights</t>
+    </r>
+  </si>
+  <si>
+    <t>These are raw numbers coming from ACS Table B08202.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are PUMS==1,2,4,5. Full distribution of households by total workers (including sick/vacationing) using person weights. Household weights yield suspect values so use person weights. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are for comparison with Columns C+D and come from PUMS data, ESR==1,4, which are workers at work (not total workers, as sick/vacationing workers are omitted). They closely match, which means B08202 is not total workers and skews the household worker distribution lower, including overrepresenting 0-worker households. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">County totals for households come from ACS Table B08202 and county worker totals come from ACS Table B23025. Total workers by household worker category (Column J) come from PUMS and are slightly rescaled to match ACS totals. Implied households are then back-calculated, starting with 3+-worker households (divided by PUMS-derived average number of workers in 3+-worker households). Two worker households are divided by 2, one divided by one, and zero is the remainder subtracted from county totals. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction factors come from dividing derived households in Column I by reported households in Column C. </t>
   </si>
 </sst>
 </file>
@@ -386,12 +476,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -551,6 +648,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1027,115 +1131,122 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1459,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,7 +1605,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="33" t="s">
         <v>52</v>
@@ -1760,80 +1871,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.58203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.58203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.58203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.08203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="31.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.08203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.58203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.75" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="31.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.08203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="261" x14ac:dyDescent="0.35">
+      <c r="C4" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="40"/>
+      <c r="K4" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38" t="s">
         <v>56</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="36" t="s">
-        <v>54</v>
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" s="37"/>
-      <c r="K5" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="19" t="s">
+      <c r="K5" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1853,272 +1978,230 @@
         <v>35</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6">
-        <v>113258</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="21">
+        <v>140827</v>
+      </c>
+      <c r="D7" s="15">
         <f>0*C7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="21">
-        <v>140827</v>
-      </c>
-      <c r="F7" s="15">
+      <c r="E7" s="6">
+        <v>143462</v>
+      </c>
+      <c r="F7" s="7">
         <f>0*E7</f>
         <v>0</v>
       </c>
       <c r="G7" s="6">
-        <v>143462</v>
+        <f>G11-SUM(G8:G10)</f>
+        <v>86733.713684844435</v>
       </c>
       <c r="H7" s="7">
         <f>0*G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="21">
         <f>I11-SUM(I8:I10)</f>
-        <v>86733.713684844435</v>
-      </c>
-      <c r="J7" s="7">
-        <f>0*I7</f>
+        <v>86035.657587368274</v>
+      </c>
+      <c r="J7" s="22">
+        <f>H7*$J$11/$H$11</f>
         <v>0</v>
       </c>
-      <c r="K7" s="21">
-        <f>K11-SUM(K8:K10)</f>
-        <v>86035.657587368274</v>
-      </c>
-      <c r="L7" s="22">
-        <f>J7*$L$11/$J$11</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="24">
-        <f>K7/E7</f>
+      <c r="K7" s="24">
+        <f>I7/C7</f>
         <v>0.61093155138835786</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16" t="s">
+      <c r="L7" s="15"/>
+      <c r="M7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="P7" s="16">
+      <c r="N7" s="16">
         <v>3.4305029999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="6">
-        <v>213454</v>
-      </c>
-      <c r="D8" s="7">
+        <v>213190</v>
+      </c>
+      <c r="D8" s="15">
         <f>1*C8</f>
-        <v>213454</v>
+        <v>213190</v>
       </c>
       <c r="E8" s="6">
-        <v>213190</v>
-      </c>
-      <c r="F8" s="15">
+        <v>211144</v>
+      </c>
+      <c r="F8" s="7">
         <f>1*E8</f>
-        <v>213190</v>
+        <v>211144</v>
       </c>
       <c r="G8" s="6">
-        <v>211144</v>
+        <f>H8/1</f>
+        <v>226429</v>
       </c>
       <c r="H8" s="7">
-        <f>1*G8</f>
-        <v>211144</v>
+        <v>226429</v>
       </c>
       <c r="I8" s="6">
         <f>J8/1</f>
-        <v>226429</v>
-      </c>
-      <c r="J8" s="7">
-        <v>226429</v>
-      </c>
-      <c r="K8" s="6">
-        <f>L8/1</f>
         <v>226757.1671019856</v>
       </c>
-      <c r="L8" s="15">
-        <f>J8*$L$11/$J$11</f>
+      <c r="J8" s="15">
+        <f>H8*$J$11/$H$11</f>
         <v>226757.1671019856</v>
       </c>
-      <c r="M8" s="25">
-        <f t="shared" ref="M8:M56" si="0">K8/E8</f>
+      <c r="K8" s="25">
+        <f t="shared" ref="K8:K56" si="0">I8/C8</f>
         <v>1.0636388531450143</v>
       </c>
-      <c r="N8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="6">
-        <v>187042</v>
-      </c>
-      <c r="D9" s="7">
+        <v>168962</v>
+      </c>
+      <c r="D9" s="15">
         <f>2*C9</f>
-        <v>374084</v>
+        <v>337924</v>
       </c>
       <c r="E9" s="6">
-        <v>168962</v>
-      </c>
-      <c r="F9" s="15">
+        <v>168189</v>
+      </c>
+      <c r="F9" s="7">
         <f>2*E9</f>
-        <v>337924</v>
+        <v>336378</v>
       </c>
       <c r="G9" s="6">
-        <v>168189</v>
+        <f>H9/2</f>
+        <v>194141</v>
       </c>
       <c r="H9" s="7">
-        <f>2*G9</f>
-        <v>336378</v>
+        <v>388282</v>
       </c>
       <c r="I9" s="6">
         <f>J9/2</f>
-        <v>194141</v>
-      </c>
-      <c r="J9" s="7">
-        <v>388282</v>
-      </c>
-      <c r="K9" s="6">
-        <f>L9/2</f>
         <v>194422.37159704184</v>
       </c>
-      <c r="L9" s="15">
-        <f>J9*$L$11/$J$11</f>
+      <c r="J9" s="15">
+        <f>H9*$J$11/$H$11</f>
         <v>388844.74319408368</v>
       </c>
-      <c r="M9" s="25">
+      <c r="K9" s="25">
         <f t="shared" si="0"/>
         <v>1.1506869686500032</v>
       </c>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="17">
-        <v>55315</v>
-      </c>
-      <c r="D10" s="18">
-        <f>C10*$P$7</f>
-        <v>189758.273445</v>
+        <v>46091</v>
+      </c>
+      <c r="D10" s="13">
+        <f>C10*$N$7</f>
+        <v>158115.313773</v>
       </c>
       <c r="E10" s="17">
-        <v>46091</v>
-      </c>
-      <c r="F10" s="13">
-        <f>E10*$P$7</f>
-        <v>158115.313773</v>
+        <v>46274</v>
+      </c>
+      <c r="F10" s="18">
+        <f>E10*$N$7</f>
+        <v>158743.095822</v>
       </c>
       <c r="G10" s="17">
-        <v>46274</v>
+        <f>H10/$N$7</f>
+        <v>61765.286315155536</v>
       </c>
       <c r="H10" s="18">
-        <f>G10*$P$7</f>
-        <v>158743.095822</v>
+        <v>211886</v>
       </c>
       <c r="I10" s="17">
-        <f>J10/$P$7</f>
-        <v>61765.286315155536</v>
-      </c>
-      <c r="J10" s="18">
-        <v>211886</v>
-      </c>
-      <c r="K10" s="17">
-        <f>L10/$P$7</f>
+        <f>J10/$N$7</f>
         <v>61854.803713604299</v>
       </c>
-      <c r="L10" s="15">
-        <f>J10*$L$11/$J$11</f>
+      <c r="J10" s="15">
+        <f>H10*$J$11/$H$11</f>
         <v>212193.08970393069</v>
       </c>
-      <c r="M10" s="26">
+      <c r="K10" s="26">
         <f t="shared" si="0"/>
         <v>1.3420147906012951</v>
       </c>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="10">
-        <f>SUM(C7:C10)</f>
+        <v>569070</v>
+      </c>
+      <c r="D11" s="14">
+        <f>SUM(D7:D10)</f>
+        <v>709229.31377300003</v>
+      </c>
+      <c r="E11" s="10">
+        <f>SUM(E7:E10)</f>
         <v>569069</v>
       </c>
-      <c r="D11" s="11">
-        <f>SUM(D7:D10)</f>
-        <v>777296.27344499994</v>
-      </c>
-      <c r="E11" s="10">
-        <v>569070</v>
-      </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <f>SUM(F7:F10)</f>
-        <v>709229.31377300003</v>
+        <v>706265.09582199994</v>
       </c>
       <c r="G11" s="10">
-        <f>SUM(G7:G10)</f>
+        <f>E11</f>
         <v>569069</v>
       </c>
       <c r="H11" s="11">
         <f>SUM(H7:H10)</f>
-        <v>706265.09582199994</v>
+        <v>826597</v>
       </c>
       <c r="I11" s="10">
         <f>C11</f>
-        <v>569069</v>
-      </c>
-      <c r="J11" s="11">
-        <f>SUM(J7:J10)</f>
-        <v>826597</v>
-      </c>
-      <c r="K11" s="10">
-        <f>E11</f>
         <v>569070</v>
       </c>
-      <c r="L11" s="14">
+      <c r="J11" s="14">
         <v>827795</v>
       </c>
-      <c r="M11" s="27">
+      <c r="K11" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2126,21 +2209,22 @@
         <v>12</v>
       </c>
       <c r="C12" s="6">
-        <v>88054</v>
-      </c>
-      <c r="D12" s="7">
+        <v>92670</v>
+      </c>
+      <c r="D12" s="15">
         <f>0*C12</f>
         <v>0</v>
       </c>
       <c r="E12" s="6">
-        <v>92670</v>
-      </c>
-      <c r="F12" s="15">
+        <v>92911</v>
+      </c>
+      <c r="F12" s="7">
         <f>0*E12</f>
         <v>0</v>
       </c>
       <c r="G12" s="6">
-        <v>92911</v>
+        <f>G16-SUM(G13:G15)</f>
+        <v>75568.145016634604</v>
       </c>
       <c r="H12" s="7">
         <f>0*G12</f>
@@ -2148,215 +2232,178 @@
       </c>
       <c r="I12" s="6">
         <f>I16-SUM(I13:I15)</f>
-        <v>75568.145016634604</v>
-      </c>
-      <c r="J12" s="7">
-        <f>0*I12</f>
+        <v>75463.451049983269</v>
+      </c>
+      <c r="J12" s="15">
+        <f>H12*$J$16/$H$16</f>
         <v>0</v>
       </c>
-      <c r="K12" s="6">
-        <f>K16-SUM(K13:K15)</f>
-        <v>75463.451049983269</v>
-      </c>
-      <c r="L12" s="15">
-        <f>J12*$L$16/$J$16</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="25">
-        <f>K12/E12</f>
+      <c r="K12" s="25">
+        <f>I12/C12</f>
         <v>0.81432449606111224</v>
       </c>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="6">
-        <v>142602</v>
-      </c>
-      <c r="D13" s="7">
+        <v>145079</v>
+      </c>
+      <c r="D13" s="15">
         <f>1*C13</f>
-        <v>142602</v>
+        <v>145079</v>
       </c>
       <c r="E13" s="6">
-        <v>145079</v>
-      </c>
-      <c r="F13" s="15">
+        <v>145632</v>
+      </c>
+      <c r="F13" s="7">
         <f>1*E13</f>
-        <v>145079</v>
+        <v>145632</v>
       </c>
       <c r="G13" s="6">
-        <v>145632</v>
+        <f>H13/1</f>
+        <v>148046</v>
       </c>
       <c r="H13" s="7">
-        <f>1*G13</f>
-        <v>145632</v>
+        <v>148046</v>
       </c>
       <c r="I13" s="6">
         <f>J13/1</f>
-        <v>148046</v>
-      </c>
-      <c r="J13" s="7">
-        <v>148046</v>
-      </c>
-      <c r="K13" s="6">
-        <f>L13/1</f>
         <v>148094.88540609516</v>
       </c>
-      <c r="L13" s="15">
-        <f>J13*$L$16/$J$16</f>
+      <c r="J13" s="15">
+        <f>H13*$J$16/$H$16</f>
         <v>148094.88540609516</v>
       </c>
-      <c r="M13" s="25">
+      <c r="K13" s="25">
         <f t="shared" si="0"/>
         <v>1.0207878838846087</v>
       </c>
-      <c r="N13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="6">
-        <v>122323</v>
-      </c>
-      <c r="D14" s="7">
+        <v>117893</v>
+      </c>
+      <c r="D14" s="15">
         <f>2*C14</f>
-        <v>244646</v>
+        <v>235786</v>
       </c>
       <c r="E14" s="6">
-        <v>117893</v>
-      </c>
-      <c r="F14" s="15">
+        <v>116594</v>
+      </c>
+      <c r="F14" s="7">
         <f>2*E14</f>
-        <v>235786</v>
+        <v>233188</v>
       </c>
       <c r="G14" s="6">
-        <v>116594</v>
+        <f>H14/2</f>
+        <v>126824</v>
       </c>
       <c r="H14" s="7">
-        <f>2*G14</f>
-        <v>233188</v>
+        <v>253648</v>
       </c>
       <c r="I14" s="6">
         <f>J14/2</f>
-        <v>126824</v>
-      </c>
-      <c r="J14" s="7">
-        <v>253648</v>
-      </c>
-      <c r="K14" s="6">
-        <f>L14/2</f>
         <v>126865.87781326487</v>
       </c>
-      <c r="L14" s="15">
-        <f>J14*$L$16/$J$16</f>
+      <c r="J14" s="15">
+        <f>H14*$J$16/$H$16</f>
         <v>253731.75562652975</v>
       </c>
-      <c r="M14" s="25">
+      <c r="K14" s="25">
         <f t="shared" si="0"/>
         <v>1.0761103527203895</v>
       </c>
-      <c r="N14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="17">
-        <v>36619</v>
-      </c>
-      <c r="D15" s="18">
-        <f>C15*$P$7</f>
-        <v>125621.58935699999</v>
+        <v>33955</v>
+      </c>
+      <c r="D15" s="13">
+        <f>C15*$N$7</f>
+        <v>116482.72936499999</v>
       </c>
       <c r="E15" s="17">
-        <v>33955</v>
-      </c>
-      <c r="F15" s="13">
-        <f>E15*$P$7</f>
-        <v>116482.72936499999</v>
+        <v>34461</v>
+      </c>
+      <c r="F15" s="18">
+        <f>E15*$N$7</f>
+        <v>118218.563883</v>
       </c>
       <c r="G15" s="17">
-        <v>34461</v>
+        <f>H15/$N$7</f>
+        <v>39159.854983365418</v>
       </c>
       <c r="H15" s="18">
-        <f>G15*$P$7</f>
-        <v>118218.563883</v>
+        <v>134338</v>
       </c>
       <c r="I15" s="17">
-        <f>J15/$P$7</f>
-        <v>39159.854983365418</v>
-      </c>
-      <c r="J15" s="18">
-        <v>134338</v>
-      </c>
-      <c r="K15" s="17">
-        <f>L15/$P$7</f>
+        <f>J15/$N$7</f>
         <v>39172.785730656724</v>
       </c>
-      <c r="L15" s="15">
-        <f>J15*$L$16/$J$16</f>
+      <c r="J15" s="15">
+        <f>H15*$J$16/$H$16</f>
         <v>134382.35896737507</v>
       </c>
-      <c r="M15" s="26">
+      <c r="K15" s="26">
         <f t="shared" si="0"/>
         <v>1.1536676698765049</v>
       </c>
-      <c r="N15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="10">
-        <f>SUM(C12:C15)</f>
+        <v>389597</v>
+      </c>
+      <c r="D16" s="14">
+        <f>SUM(D12:D15)</f>
+        <v>497347.72936499998</v>
+      </c>
+      <c r="E16" s="10">
+        <f>SUM(E12:E15)</f>
         <v>389598</v>
       </c>
-      <c r="D16" s="11">
-        <f>SUM(D12:D15)</f>
-        <v>512869.58935699996</v>
-      </c>
-      <c r="E16" s="10">
-        <v>389597</v>
-      </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <f>SUM(F12:F15)</f>
-        <v>497347.72936499998</v>
+        <v>497038.563883</v>
       </c>
       <c r="G16" s="10">
-        <f>SUM(G12:G15)</f>
+        <f>E16</f>
         <v>389598</v>
       </c>
       <c r="H16" s="11">
         <f>SUM(H12:H15)</f>
-        <v>497038.563883</v>
+        <v>536032</v>
       </c>
       <c r="I16" s="10">
         <f>C16</f>
-        <v>389598</v>
-      </c>
-      <c r="J16" s="11">
-        <f>SUM(J12:J15)</f>
-        <v>536032</v>
-      </c>
-      <c r="K16" s="10">
-        <f>E16</f>
         <v>389597</v>
       </c>
-      <c r="L16" s="14">
+      <c r="J16" s="14">
         <v>536209</v>
       </c>
-      <c r="M16" s="27">
+      <c r="K16" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2364,21 +2411,22 @@
         <v>12</v>
       </c>
       <c r="C17" s="6">
-        <v>26688</v>
-      </c>
-      <c r="D17" s="7">
+        <v>27347</v>
+      </c>
+      <c r="D17" s="15">
         <f>0*C17</f>
         <v>0</v>
       </c>
       <c r="E17" s="6">
-        <v>27347</v>
-      </c>
-      <c r="F17" s="15">
+        <v>27724</v>
+      </c>
+      <c r="F17" s="7">
         <f>0*E17</f>
         <v>0</v>
       </c>
       <c r="G17" s="6">
-        <v>27724</v>
+        <f>G21-SUM(G18:G20)</f>
+        <v>23050.232510072135</v>
       </c>
       <c r="H17" s="7">
         <f>0*G17</f>
@@ -2386,216 +2434,179 @@
       </c>
       <c r="I17" s="6">
         <f>I21-SUM(I18:I20)</f>
-        <v>23050.232510072135</v>
-      </c>
-      <c r="J17" s="7">
-        <f>0*I17</f>
+        <v>22411.547874839292</v>
+      </c>
+      <c r="J17" s="15">
+        <f>H17*$J$21/$H$21</f>
         <v>0</v>
       </c>
-      <c r="K17" s="6">
-        <f>K21-SUM(K18:K20)</f>
-        <v>22411.547874839292</v>
-      </c>
-      <c r="L17" s="15">
-        <f>J17*$L$21/$J$21</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="25">
-        <f>K17/E17</f>
+      <c r="K17" s="25">
+        <f>I17/C17</f>
         <v>0.81952491588983412</v>
       </c>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="6">
-        <v>41397</v>
-      </c>
-      <c r="D18" s="7">
+        <v>41727</v>
+      </c>
+      <c r="D18" s="15">
         <f>1*C18</f>
-        <v>41397</v>
+        <v>41727</v>
       </c>
       <c r="E18" s="6">
-        <v>41727</v>
-      </c>
-      <c r="F18" s="15">
+        <v>41600</v>
+      </c>
+      <c r="F18" s="7">
         <f>1*E18</f>
-        <v>41727</v>
+        <v>41600</v>
       </c>
       <c r="G18" s="6">
-        <v>41600</v>
+        <f>H18/1</f>
+        <v>43335</v>
       </c>
       <c r="H18" s="7">
-        <f>1*G18</f>
-        <v>41600</v>
+        <v>43335</v>
       </c>
       <c r="I18" s="6">
         <f>J18/1</f>
-        <v>43335</v>
-      </c>
-      <c r="J18" s="7">
-        <v>43335</v>
-      </c>
-      <c r="K18" s="6">
-        <f>L18/1</f>
         <v>43673.372015046174</v>
       </c>
-      <c r="L18" s="15">
-        <f>J18*$L$21/$J$21</f>
+      <c r="J18" s="15">
+        <f>H18*$J$21/$H$21</f>
         <v>43673.372015046174</v>
       </c>
-      <c r="M18" s="25">
+      <c r="K18" s="25">
         <f t="shared" si="0"/>
         <v>1.0466453858424083</v>
       </c>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="6">
-        <v>30725</v>
-      </c>
-      <c r="D19" s="7">
+        <v>30126</v>
+      </c>
+      <c r="D19" s="15">
         <f>2*C19</f>
-        <v>61450</v>
+        <v>60252</v>
       </c>
       <c r="E19" s="6">
-        <v>30126</v>
-      </c>
-      <c r="F19" s="15">
+        <v>29864</v>
+      </c>
+      <c r="F19" s="7">
         <f>2*E19</f>
-        <v>60252</v>
+        <v>59728</v>
       </c>
       <c r="G19" s="6">
-        <v>29864</v>
+        <f>H19/2</f>
+        <v>31835.5</v>
       </c>
       <c r="H19" s="7">
-        <f>2*G19</f>
-        <v>59728</v>
+        <v>63671</v>
       </c>
       <c r="I19" s="6">
         <f>J19/2</f>
-        <v>31835.5</v>
-      </c>
-      <c r="J19" s="7">
-        <v>63671</v>
-      </c>
-      <c r="K19" s="6">
-        <f>L19/2</f>
         <v>32084.080645782909</v>
       </c>
-      <c r="L19" s="15">
-        <f>J19*$L$21/$J$21</f>
+      <c r="J19" s="15">
+        <f>H19*$J$21/$H$21</f>
         <v>64168.161291565819</v>
       </c>
-      <c r="M19" s="25">
+      <c r="K19" s="25">
         <f t="shared" si="0"/>
         <v>1.0649963701049894</v>
       </c>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="17">
-        <v>6036</v>
-      </c>
-      <c r="D20" s="18">
-        <f>C20*$P$7</f>
-        <v>20706.516108</v>
+        <v>5646</v>
+      </c>
+      <c r="D20" s="13">
+        <f>C20*$N$7</f>
+        <v>19368.619938</v>
       </c>
       <c r="E20" s="17">
-        <v>5646</v>
-      </c>
-      <c r="F20" s="13">
-        <f>E20*$P$7</f>
-        <v>19368.619938</v>
+        <v>5658</v>
+      </c>
+      <c r="F20" s="18">
+        <f>E20*$N$7</f>
+        <v>19409.785973999999</v>
       </c>
       <c r="G20" s="17">
-        <v>5658</v>
+        <f>H20/$N$7</f>
+        <v>6625.2674899278618</v>
       </c>
       <c r="H20" s="18">
-        <f>G20*$P$7</f>
-        <v>19409.785973999999</v>
+        <v>22728</v>
       </c>
       <c r="I20" s="17">
-        <f>J20/$P$7</f>
-        <v>6625.2674899278618</v>
-      </c>
-      <c r="J20" s="18">
-        <v>22728</v>
-      </c>
-      <c r="K20" s="17">
-        <f>L20/$P$7</f>
+        <f>J20/$N$7</f>
         <v>6676.9994643316186</v>
       </c>
-      <c r="L20" s="15">
-        <f>J20*$L$21/$J$21</f>
+      <c r="J20" s="15">
+        <f>H20*$J$21/$H$21</f>
         <v>22905.466693388011</v>
       </c>
-      <c r="M20" s="26">
+      <c r="K20" s="26">
         <f t="shared" si="0"/>
         <v>1.1826070606325927</v>
       </c>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="10">
-        <f>SUM(C17:C20)</f>
         <v>104846</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="14">
         <f>SUM(D17:D20)</f>
-        <v>123553.516108</v>
+        <v>121347.619938</v>
       </c>
       <c r="E21" s="10">
+        <f>SUM(E17:E20)</f>
         <v>104846</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <f>SUM(F17:F20)</f>
-        <v>121347.619938</v>
+        <v>120737.785974</v>
       </c>
       <c r="G21" s="10">
-        <f>SUM(G17:G20)</f>
+        <f>E21</f>
         <v>104846</v>
       </c>
       <c r="H21" s="11">
         <f>SUM(H17:H20)</f>
-        <v>120737.785974</v>
+        <v>129734</v>
       </c>
       <c r="I21" s="10">
         <f>C21</f>
         <v>104846</v>
       </c>
-      <c r="J21" s="11">
-        <f>SUM(J17:J20)</f>
-        <v>129734</v>
-      </c>
-      <c r="K21" s="10">
-        <f>E21</f>
-        <v>104846</v>
-      </c>
-      <c r="L21" s="14">
+      <c r="J21" s="14">
         <v>130747</v>
       </c>
-      <c r="M21" s="27">
+      <c r="K21" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2603,21 +2614,22 @@
         <v>12</v>
       </c>
       <c r="C22" s="6">
-        <v>12334</v>
-      </c>
-      <c r="D22" s="7">
+        <v>12572</v>
+      </c>
+      <c r="D22" s="15">
         <f>0*C22</f>
         <v>0</v>
       </c>
       <c r="E22" s="6">
-        <v>12572</v>
-      </c>
-      <c r="F22" s="15">
+        <v>12761</v>
+      </c>
+      <c r="F22" s="7">
         <f>0*E22</f>
         <v>0</v>
       </c>
       <c r="G22" s="6">
-        <v>12761</v>
+        <f>G26-SUM(G23:G25)</f>
+        <v>8828.9756865101081</v>
       </c>
       <c r="H22" s="7">
         <f>0*G22</f>
@@ -2625,215 +2637,178 @@
       </c>
       <c r="I22" s="6">
         <f>I26-SUM(I23:I25)</f>
-        <v>8828.9756865101081</v>
-      </c>
-      <c r="J22" s="7">
-        <f>0*I22</f>
+        <v>8929.3384581970749</v>
+      </c>
+      <c r="J22" s="15">
+        <f>H22*$J$26/$H$26</f>
         <v>0</v>
       </c>
-      <c r="K22" s="6">
-        <f>K26-SUM(K23:K25)</f>
-        <v>8929.3384581970749</v>
-      </c>
-      <c r="L22" s="15">
-        <f>J22*$L$26/$J$26</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="25">
-        <f>K22/E22</f>
+      <c r="K22" s="25">
+        <f>I22/C22</f>
         <v>0.71025600208376349</v>
       </c>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="6">
-        <v>15947</v>
-      </c>
-      <c r="D23" s="7">
+        <v>16470</v>
+      </c>
+      <c r="D23" s="15">
         <f>1*C23</f>
-        <v>15947</v>
+        <v>16470</v>
       </c>
       <c r="E23" s="6">
-        <v>16470</v>
-      </c>
-      <c r="F23" s="15">
+        <v>16310</v>
+      </c>
+      <c r="F23" s="7">
         <f>1*E23</f>
-        <v>16470</v>
+        <v>16310</v>
       </c>
       <c r="G23" s="6">
-        <v>16310</v>
+        <f>H23/1</f>
+        <v>17614</v>
       </c>
       <c r="H23" s="7">
-        <f>1*G23</f>
-        <v>16310</v>
+        <v>17614</v>
       </c>
       <c r="I23" s="6">
         <f>J23/1</f>
-        <v>17614</v>
-      </c>
-      <c r="J23" s="7">
-        <v>17614</v>
-      </c>
-      <c r="K23" s="6">
-        <f>L23/1</f>
         <v>17570.041556839213</v>
       </c>
-      <c r="L23" s="15">
-        <f>J23*$L$26/$J$26</f>
+      <c r="J23" s="15">
+        <f>H23*$J$26/$H$26</f>
         <v>17570.041556839213</v>
       </c>
-      <c r="M23" s="25">
+      <c r="K23" s="25">
         <f t="shared" si="0"/>
         <v>1.0667906227589079</v>
       </c>
-      <c r="N23" s="15"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="6">
-        <v>15628</v>
-      </c>
-      <c r="D24" s="7">
+        <v>15313</v>
+      </c>
+      <c r="D24" s="15">
         <f>2*C24</f>
-        <v>31256</v>
+        <v>30626</v>
       </c>
       <c r="E24" s="6">
-        <v>15313</v>
-      </c>
-      <c r="F24" s="15">
+        <v>15169</v>
+      </c>
+      <c r="F24" s="7">
         <f>2*E24</f>
-        <v>30626</v>
+        <v>30338</v>
       </c>
       <c r="G24" s="6">
-        <v>15169</v>
+        <f>H24/2</f>
+        <v>16653.5</v>
       </c>
       <c r="H24" s="7">
-        <f>2*G24</f>
-        <v>30338</v>
+        <v>33307</v>
       </c>
       <c r="I24" s="6">
         <f>J24/2</f>
-        <v>16653.5</v>
-      </c>
-      <c r="J24" s="7">
-        <v>33307</v>
-      </c>
-      <c r="K24" s="6">
-        <f>L24/2</f>
         <v>16611.938632157478</v>
       </c>
-      <c r="L24" s="15">
-        <f>J24*$L$26/$J$26</f>
+      <c r="J24" s="15">
+        <f>H24*$J$26/$H$26</f>
         <v>33223.877264314957</v>
       </c>
-      <c r="M24" s="25">
+      <c r="K24" s="25">
         <f t="shared" si="0"/>
         <v>1.0848258755408788</v>
       </c>
-      <c r="N24" s="15"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="17">
-        <v>5135</v>
-      </c>
-      <c r="D25" s="18">
-        <f>C25*$P$7</f>
-        <v>17615.632904999999</v>
+        <v>4689</v>
+      </c>
+      <c r="D25" s="13">
+        <f>C25*$N$7</f>
+        <v>16085.628567</v>
       </c>
       <c r="E25" s="17">
-        <v>4689</v>
-      </c>
-      <c r="F25" s="13">
-        <f>E25*$P$7</f>
-        <v>16085.628567</v>
+        <v>4804</v>
+      </c>
+      <c r="F25" s="18">
+        <f>E25*$N$7</f>
+        <v>16480.136412</v>
       </c>
       <c r="G25" s="17">
-        <v>4804</v>
+        <f>H25/$N$7</f>
+        <v>5947.5243134898883</v>
       </c>
       <c r="H25" s="18">
-        <f>G25*$P$7</f>
-        <v>16480.136412</v>
+        <v>20403</v>
       </c>
       <c r="I25" s="17">
-        <f>J25/$P$7</f>
-        <v>5947.5243134898883</v>
-      </c>
-      <c r="J25" s="18">
-        <v>20403</v>
-      </c>
-      <c r="K25" s="17">
-        <f>L25/$P$7</f>
+        <f>J25/$N$7</f>
         <v>5932.6813528062303</v>
       </c>
-      <c r="L25" s="15">
-        <f>J25*$L$26/$J$26</f>
+      <c r="J25" s="15">
+        <f>H25*$J$26/$H$26</f>
         <v>20352.08117884583</v>
       </c>
-      <c r="M25" s="26">
+      <c r="K25" s="26">
         <f t="shared" si="0"/>
         <v>1.2652338137782535</v>
       </c>
-      <c r="N25" s="15"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="10">
-        <f>SUM(C22:C25)</f>
         <v>49044</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="14">
         <f>SUM(D22:D25)</f>
-        <v>64818.632904999999</v>
+        <v>63181.628567</v>
       </c>
       <c r="E26" s="10">
+        <f>SUM(E22:E25)</f>
         <v>49044</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="11">
         <f>SUM(F22:F25)</f>
-        <v>63181.628567</v>
+        <v>63128.136412</v>
       </c>
       <c r="G26" s="10">
-        <f>SUM(G22:G25)</f>
+        <f>E26</f>
         <v>49044</v>
       </c>
       <c r="H26" s="11">
         <f>SUM(H22:H25)</f>
-        <v>63128.136412</v>
+        <v>71324</v>
       </c>
       <c r="I26" s="10">
         <f>C26</f>
         <v>49044</v>
       </c>
-      <c r="J26" s="11">
-        <f>SUM(J22:J25)</f>
-        <v>71324</v>
-      </c>
-      <c r="K26" s="10">
-        <f>E26</f>
-        <v>49044</v>
-      </c>
-      <c r="L26" s="14">
+      <c r="J26" s="14">
         <v>71146</v>
       </c>
-      <c r="M26" s="27">
+      <c r="K26" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N26" s="15"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -2841,21 +2816,22 @@
         <v>12</v>
       </c>
       <c r="C27" s="6">
-        <v>78264</v>
-      </c>
-      <c r="D27" s="7">
+        <v>82119</v>
+      </c>
+      <c r="D27" s="15">
         <f>0*C27</f>
         <v>0</v>
       </c>
       <c r="E27" s="6">
-        <v>82119</v>
-      </c>
-      <c r="F27" s="15">
+        <v>81411</v>
+      </c>
+      <c r="F27" s="7">
         <f>0*E27</f>
         <v>0</v>
       </c>
       <c r="G27" s="6">
-        <v>81411</v>
+        <f>G31-SUM(G28:G30)</f>
+        <v>59260.339867069037</v>
       </c>
       <c r="H27" s="7">
         <f>0*G27</f>
@@ -2863,215 +2839,178 @@
       </c>
       <c r="I27" s="6">
         <f>I31-SUM(I28:I30)</f>
-        <v>59260.339867069037</v>
-      </c>
-      <c r="J27" s="7">
-        <f>0*I27</f>
+        <v>59486.398252129438</v>
+      </c>
+      <c r="J27" s="15">
+        <f>H27*$J$31/$H$31</f>
         <v>0</v>
       </c>
-      <c r="K27" s="6">
-        <f>K31-SUM(K28:K30)</f>
-        <v>59486.398252129438</v>
-      </c>
-      <c r="L27" s="15">
-        <f>J27*$L$31/$J$31</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="25">
-        <f>K27/E27</f>
+      <c r="K27" s="25">
+        <f>I27/C27</f>
         <v>0.7243926284066956</v>
       </c>
-      <c r="N27" s="15"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="6">
-        <v>138821</v>
-      </c>
-      <c r="D28" s="7">
+        <v>139605</v>
+      </c>
+      <c r="D28" s="15">
         <f>1*C28</f>
-        <v>138821</v>
+        <v>139605</v>
       </c>
       <c r="E28" s="6">
-        <v>139605</v>
-      </c>
-      <c r="F28" s="15">
+        <v>140358</v>
+      </c>
+      <c r="F28" s="7">
         <f>1*E28</f>
-        <v>139605</v>
+        <v>140358</v>
       </c>
       <c r="G28" s="6">
-        <v>140358</v>
+        <f>H28/1</f>
+        <v>147392</v>
       </c>
       <c r="H28" s="7">
-        <f>1*G28</f>
-        <v>140358</v>
+        <v>147392</v>
       </c>
       <c r="I28" s="6">
         <f>J28/1</f>
-        <v>147392</v>
-      </c>
-      <c r="J28" s="7">
-        <v>147392</v>
-      </c>
-      <c r="K28" s="6">
-        <f>L28/1</f>
         <v>147281.24666161765</v>
       </c>
-      <c r="L28" s="15">
-        <f>J28*$L$31/$J$31</f>
+      <c r="J28" s="15">
+        <f>H28*$J$31/$H$31</f>
         <v>147281.24666161765</v>
       </c>
-      <c r="M28" s="25">
+      <c r="K28" s="25">
         <f t="shared" si="0"/>
         <v>1.0549854708758115</v>
       </c>
-      <c r="N28" s="15"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L28" s="15"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="6">
-        <v>109609</v>
-      </c>
-      <c r="D29" s="7">
+        <v>106022</v>
+      </c>
+      <c r="D29" s="15">
         <f>2*C29</f>
-        <v>219218</v>
+        <v>212044</v>
       </c>
       <c r="E29" s="6">
-        <v>106022</v>
-      </c>
-      <c r="F29" s="15">
+        <v>105837</v>
+      </c>
+      <c r="F29" s="7">
         <f>2*E29</f>
-        <v>212044</v>
+        <v>211674</v>
       </c>
       <c r="G29" s="6">
-        <v>105837</v>
+        <f>H29/2</f>
+        <v>114314</v>
       </c>
       <c r="H29" s="7">
-        <f>2*G29</f>
-        <v>211674</v>
+        <v>228628</v>
       </c>
       <c r="I29" s="6">
         <f>J29/2</f>
-        <v>114314</v>
-      </c>
-      <c r="J29" s="7">
-        <v>228628</v>
-      </c>
-      <c r="K29" s="6">
-        <f>L29/2</f>
         <v>114228.10214174555</v>
       </c>
-      <c r="L29" s="15">
-        <f>J29*$L$31/$J$31</f>
+      <c r="J29" s="15">
+        <f>H29*$J$31/$H$31</f>
         <v>228456.2042834911</v>
       </c>
-      <c r="M29" s="25">
+      <c r="K29" s="25">
         <f t="shared" si="0"/>
         <v>1.077399993791341</v>
       </c>
-      <c r="N29" s="15"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L29" s="15"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="17">
-        <v>32077</v>
-      </c>
-      <c r="D30" s="18">
-        <f>C30*$P$7</f>
-        <v>110040.244731</v>
+        <v>31026</v>
+      </c>
+      <c r="D30" s="13">
+        <f>C30*$N$7</f>
+        <v>106434.78607799999</v>
       </c>
       <c r="E30" s="17">
-        <v>31026</v>
-      </c>
-      <c r="F30" s="13">
-        <f>E30*$P$7</f>
-        <v>106434.78607799999</v>
+        <v>31165</v>
+      </c>
+      <c r="F30" s="18">
+        <f>E30*$N$7</f>
+        <v>106911.62599499999</v>
       </c>
       <c r="G30" s="17">
-        <v>31165</v>
+        <f>H30/$N$7</f>
+        <v>37804.660132930941</v>
       </c>
       <c r="H30" s="18">
-        <f>G30*$P$7</f>
-        <v>106911.62599499999</v>
+        <v>129689</v>
       </c>
       <c r="I30" s="17">
-        <f>J30/$P$7</f>
-        <v>37804.660132930941</v>
-      </c>
-      <c r="J30" s="18">
-        <v>129689</v>
-      </c>
-      <c r="K30" s="17">
-        <f>L30/$P$7</f>
+        <f>J30/$N$7</f>
         <v>37776.252944507338</v>
       </c>
-      <c r="L30" s="15">
-        <f>J30*$L$31/$J$31</f>
+      <c r="J30" s="15">
+        <f>H30*$J$31/$H$31</f>
         <v>129591.54905489125</v>
       </c>
-      <c r="M30" s="26">
+      <c r="K30" s="26">
         <f t="shared" si="0"/>
         <v>1.2175676189166291</v>
       </c>
-      <c r="N30" s="15"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="10">
-        <f>SUM(C27:C30)</f>
+        <v>358772</v>
+      </c>
+      <c r="D31" s="14">
+        <f>SUM(D27:D30)</f>
+        <v>458083.78607799998</v>
+      </c>
+      <c r="E31" s="10">
+        <f>SUM(E27:E30)</f>
         <v>358771</v>
       </c>
-      <c r="D31" s="11">
-        <f>SUM(D27:D30)</f>
-        <v>468079.24473099998</v>
-      </c>
-      <c r="E31" s="10">
-        <v>358772</v>
-      </c>
-      <c r="F31" s="14">
+      <c r="F31" s="11">
         <f>SUM(F27:F30)</f>
-        <v>458083.78607799998</v>
+        <v>458943.62599500001</v>
       </c>
       <c r="G31" s="10">
-        <f>SUM(G27:G30)</f>
+        <f>E31</f>
         <v>358771</v>
       </c>
       <c r="H31" s="11">
         <f>SUM(H27:H30)</f>
-        <v>458943.62599500001</v>
+        <v>505709</v>
       </c>
       <c r="I31" s="10">
         <f>C31</f>
-        <v>358771</v>
-      </c>
-      <c r="J31" s="11">
-        <f>SUM(J27:J30)</f>
-        <v>505709</v>
-      </c>
-      <c r="K31" s="10">
-        <f>E31</f>
         <v>358772</v>
       </c>
-      <c r="L31" s="14">
+      <c r="J31" s="14">
         <v>505329</v>
       </c>
-      <c r="M31" s="27">
+      <c r="K31" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N31" s="15"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -3079,21 +3018,22 @@
         <v>12</v>
       </c>
       <c r="C32" s="6">
-        <v>48552</v>
-      </c>
-      <c r="D32" s="7">
+        <v>50750</v>
+      </c>
+      <c r="D32" s="15">
         <f>0*C32</f>
         <v>0</v>
       </c>
       <c r="E32" s="6">
-        <v>50750</v>
-      </c>
-      <c r="F32" s="15">
+        <v>50939</v>
+      </c>
+      <c r="F32" s="7">
         <f>0*E32</f>
         <v>0</v>
       </c>
       <c r="G32" s="6">
-        <v>50939</v>
+        <f>G36-SUM(G33:G35)</f>
+        <v>35819.133165019826</v>
       </c>
       <c r="H32" s="7">
         <f>0*G32</f>
@@ -3101,215 +3041,178 @@
       </c>
       <c r="I32" s="6">
         <f>I36-SUM(I33:I35)</f>
-        <v>35819.133165019826</v>
-      </c>
-      <c r="J32" s="7">
-        <f>0*I32</f>
+        <v>36055.571486832458</v>
+      </c>
+      <c r="J32" s="15">
+        <f>H32*$J$36/$H$36</f>
         <v>0</v>
       </c>
-      <c r="K32" s="6">
-        <f>K36-SUM(K33:K35)</f>
-        <v>36055.571486832458</v>
-      </c>
-      <c r="L32" s="15">
-        <f>J32*$L$36/$J$36</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="25">
-        <f>K32/E32</f>
+      <c r="K32" s="25">
+        <f>I32/C32</f>
         <v>0.71045461057797943</v>
       </c>
-      <c r="N32" s="15"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="6">
-        <v>92435</v>
-      </c>
-      <c r="D33" s="7">
+        <v>95393</v>
+      </c>
+      <c r="D33" s="15">
         <f>1*C33</f>
-        <v>92435</v>
+        <v>95393</v>
       </c>
       <c r="E33" s="6">
-        <v>95393</v>
-      </c>
-      <c r="F33" s="15">
+        <v>94041</v>
+      </c>
+      <c r="F33" s="7">
         <f>1*E33</f>
-        <v>95393</v>
+        <v>94041</v>
       </c>
       <c r="G33" s="6">
-        <v>94041</v>
+        <f>H33/1</f>
+        <v>97044</v>
       </c>
       <c r="H33" s="7">
-        <f>1*G33</f>
-        <v>94041</v>
+        <v>97044</v>
       </c>
       <c r="I33" s="6">
         <f>J33/1</f>
-        <v>97044</v>
-      </c>
-      <c r="J33" s="7">
-        <v>97044</v>
-      </c>
-      <c r="K33" s="6">
-        <f>L33/1</f>
         <v>96943.750405569997</v>
       </c>
-      <c r="L33" s="15">
-        <f>J33*$L$36/$J$36</f>
+      <c r="J33" s="15">
+        <f>H33*$J$36/$H$36</f>
         <v>96943.750405569997</v>
       </c>
-      <c r="M33" s="25">
+      <c r="K33" s="25">
         <f t="shared" si="0"/>
         <v>1.0162564381618149</v>
       </c>
-      <c r="N33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="6">
-        <v>90081</v>
-      </c>
-      <c r="D34" s="7">
+        <v>86422</v>
+      </c>
+      <c r="D34" s="15">
         <f>2*C34</f>
-        <v>180162</v>
+        <v>172844</v>
       </c>
       <c r="E34" s="6">
-        <v>86422</v>
-      </c>
-      <c r="F34" s="15">
+        <v>87327</v>
+      </c>
+      <c r="F34" s="7">
         <f>2*E34</f>
-        <v>172844</v>
+        <v>174654</v>
       </c>
       <c r="G34" s="6">
-        <v>87327</v>
+        <f>H34/2</f>
+        <v>93489</v>
       </c>
       <c r="H34" s="7">
-        <f>2*G34</f>
-        <v>174654</v>
+        <v>186978</v>
       </c>
       <c r="I34" s="6">
         <f>J34/2</f>
-        <v>93489</v>
-      </c>
-      <c r="J34" s="7">
-        <v>186978</v>
-      </c>
-      <c r="K34" s="6">
-        <f>L34/2</f>
         <v>93392.422835686215</v>
       </c>
-      <c r="L34" s="15">
-        <f>J34*$L$36/$J$36</f>
+      <c r="J34" s="15">
+        <f>H34*$J$36/$H$36</f>
         <v>186784.84567137243</v>
       </c>
-      <c r="M34" s="25">
+      <c r="K34" s="25">
         <f t="shared" si="0"/>
         <v>1.080655652908822</v>
       </c>
-      <c r="N34" s="15"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="17">
-        <v>30725</v>
-      </c>
-      <c r="D35" s="18">
-        <f>C35*$P$7</f>
-        <v>105402.204675</v>
+        <v>29231</v>
+      </c>
+      <c r="D35" s="13">
+        <f>C35*$N$7</f>
+        <v>100277.033193</v>
       </c>
       <c r="E35" s="17">
-        <v>29231</v>
-      </c>
-      <c r="F35" s="13">
-        <f>E35*$P$7</f>
-        <v>100277.033193</v>
+        <v>29486</v>
+      </c>
+      <c r="F35" s="18">
+        <f>E35*$N$7</f>
+        <v>101151.811458</v>
       </c>
       <c r="G35" s="17">
-        <v>29486</v>
+        <f>H35/$N$7</f>
+        <v>35440.866834980181</v>
       </c>
       <c r="H35" s="18">
-        <f>G35*$P$7</f>
-        <v>101151.811458</v>
+        <v>121580</v>
       </c>
       <c r="I35" s="17">
-        <f>J35/$P$7</f>
-        <v>35440.866834980181</v>
-      </c>
-      <c r="J35" s="18">
-        <v>121580</v>
-      </c>
-      <c r="K35" s="17">
-        <f>L35/$P$7</f>
+        <f>J35/$N$7</f>
         <v>35404.255271911316</v>
       </c>
-      <c r="L35" s="15">
-        <f>J35*$L$36/$J$36</f>
+      <c r="J35" s="15">
+        <f>H35*$J$36/$H$36</f>
         <v>121454.40392305757</v>
       </c>
-      <c r="M35" s="26">
+      <c r="K35" s="26">
         <f t="shared" si="0"/>
         <v>1.2111886446550346</v>
       </c>
-      <c r="N35" s="15"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="10">
-        <f>SUM(C32:C35)</f>
+        <v>261796</v>
+      </c>
+      <c r="D36" s="14">
+        <f>SUM(D32:D35)</f>
+        <v>368514.03319300001</v>
+      </c>
+      <c r="E36" s="10">
+        <f>SUM(E32:E35)</f>
         <v>261793</v>
       </c>
-      <c r="D36" s="11">
-        <f>SUM(D32:D35)</f>
-        <v>377999.20467499999</v>
-      </c>
-      <c r="E36" s="10">
-        <v>261796</v>
-      </c>
-      <c r="F36" s="14">
+      <c r="F36" s="11">
         <f>SUM(F32:F35)</f>
-        <v>368514.03319300001</v>
+        <v>369846.81145799998</v>
       </c>
       <c r="G36" s="10">
-        <f>SUM(G32:G35)</f>
+        <f>E36</f>
         <v>261793</v>
       </c>
       <c r="H36" s="11">
         <f>SUM(H32:H35)</f>
-        <v>369846.81145799998</v>
+        <v>405602</v>
       </c>
       <c r="I36" s="10">
         <f>C36</f>
-        <v>261793</v>
-      </c>
-      <c r="J36" s="11">
-        <f>SUM(J32:J35)</f>
-        <v>405602</v>
-      </c>
-      <c r="K36" s="10">
-        <f>E36</f>
         <v>261796</v>
       </c>
-      <c r="L36" s="14">
+      <c r="J36" s="14">
         <v>405183</v>
       </c>
-      <c r="M36" s="27">
+      <c r="K36" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N36" s="15"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -3317,21 +3220,22 @@
         <v>12</v>
       </c>
       <c r="C37" s="6">
-        <v>108266</v>
-      </c>
-      <c r="D37" s="7">
+        <v>118875</v>
+      </c>
+      <c r="D37" s="15">
         <f>0*C37</f>
         <v>0</v>
       </c>
       <c r="E37" s="6">
-        <v>118875</v>
-      </c>
-      <c r="F37" s="15">
+        <v>118258</v>
+      </c>
+      <c r="F37" s="7">
         <f>0*E37</f>
         <v>0</v>
       </c>
       <c r="G37" s="6">
-        <v>118258</v>
+        <f>G41-SUM(G38:G40)</f>
+        <v>77161.554665744305</v>
       </c>
       <c r="H37" s="7">
         <f>0*G37</f>
@@ -3339,215 +3243,178 @@
       </c>
       <c r="I37" s="6">
         <f>I41-SUM(I38:I40)</f>
-        <v>77161.554665744305</v>
-      </c>
-      <c r="J37" s="7">
-        <f>0*I37</f>
+        <v>77547.441707691876</v>
+      </c>
+      <c r="J37" s="15">
+        <f>H37*$J$41/$H$41</f>
         <v>0</v>
       </c>
-      <c r="K37" s="6">
-        <f>K41-SUM(K38:K40)</f>
-        <v>77547.441707691876</v>
-      </c>
-      <c r="L37" s="15">
-        <f>J37*$L$41/$J$41</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="25">
-        <f>K37/E37</f>
+      <c r="K37" s="25">
+        <f>I37/C37</f>
         <v>0.65234440973873298</v>
       </c>
-      <c r="N37" s="15"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L37" s="15"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="6">
-        <v>238446</v>
-      </c>
-      <c r="D38" s="7">
+        <v>240595</v>
+      </c>
+      <c r="D38" s="15">
         <f>1*C38</f>
-        <v>238446</v>
+        <v>240595</v>
       </c>
       <c r="E38" s="6">
-        <v>240595</v>
-      </c>
-      <c r="F38" s="15">
+        <v>241135</v>
+      </c>
+      <c r="F38" s="7">
         <f>1*E38</f>
-        <v>240595</v>
+        <v>241135</v>
       </c>
       <c r="G38" s="6">
-        <v>241135</v>
+        <f>H38/1</f>
+        <v>252019</v>
       </c>
       <c r="H38" s="7">
-        <f>1*G38</f>
-        <v>241135</v>
+        <v>252019</v>
       </c>
       <c r="I38" s="6">
         <f>J38/1</f>
-        <v>252019</v>
-      </c>
-      <c r="J38" s="7">
-        <v>252019</v>
-      </c>
-      <c r="K38" s="6">
-        <f>L38/1</f>
         <v>251842.32113527344</v>
       </c>
-      <c r="L38" s="15">
-        <f>J38*$L$41/$J$41</f>
+      <c r="J38" s="15">
+        <f>H38*$J$41/$H$41</f>
         <v>251842.32113527344</v>
       </c>
-      <c r="M38" s="25">
+      <c r="K38" s="25">
         <f t="shared" si="0"/>
         <v>1.0467479421237909</v>
       </c>
-      <c r="N38" s="15"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L38" s="15"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C39" s="6">
-        <v>214043</v>
-      </c>
-      <c r="D39" s="7">
+        <v>204894</v>
+      </c>
+      <c r="D39" s="15">
         <f>2*C39</f>
-        <v>428086</v>
+        <v>409788</v>
       </c>
       <c r="E39" s="6">
-        <v>204894</v>
-      </c>
-      <c r="F39" s="15">
+        <v>205440</v>
+      </c>
+      <c r="F39" s="7">
         <f>2*E39</f>
-        <v>409788</v>
+        <v>410880</v>
       </c>
       <c r="G39" s="6">
-        <v>205440</v>
+        <f>H39/2</f>
+        <v>221595.5</v>
       </c>
       <c r="H39" s="7">
-        <f>2*G39</f>
-        <v>410880</v>
+        <v>443191</v>
       </c>
       <c r="I39" s="6">
         <f>J39/2</f>
-        <v>221595.5</v>
-      </c>
-      <c r="J39" s="7">
-        <v>443191</v>
-      </c>
-      <c r="K39" s="6">
-        <f>L39/2</f>
         <v>221440.14964400098</v>
       </c>
-      <c r="L39" s="15">
-        <f>J39*$L$41/$J$41</f>
+      <c r="J39" s="15">
+        <f>H39*$J$41/$H$41</f>
         <v>442880.29928800196</v>
       </c>
-      <c r="M39" s="25">
+      <c r="K39" s="25">
         <f t="shared" si="0"/>
         <v>1.0807546811717326</v>
       </c>
-      <c r="N39" s="15"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L39" s="15"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="12"/>
       <c r="B40" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="17">
-        <v>69698</v>
-      </c>
-      <c r="D40" s="18">
-        <f>C40*$P$7</f>
-        <v>239099.19809399999</v>
+        <v>66087</v>
+      </c>
+      <c r="D40" s="13">
+        <f>C40*$N$7</f>
+        <v>226711.65176099999</v>
       </c>
       <c r="E40" s="17">
-        <v>66087</v>
-      </c>
-      <c r="F40" s="13">
-        <f>E40*$P$7</f>
-        <v>226711.65176099999</v>
+        <v>65620</v>
+      </c>
+      <c r="F40" s="18">
+        <f>E40*$N$7</f>
+        <v>225109.60686</v>
       </c>
       <c r="G40" s="17">
-        <v>65620</v>
+        <f>H40/$N$7</f>
+        <v>79676.945334255652</v>
       </c>
       <c r="H40" s="18">
-        <f>G40*$P$7</f>
-        <v>225109.60686</v>
+        <v>273332</v>
       </c>
       <c r="I40" s="17">
-        <f>J40/$P$7</f>
-        <v>79676.945334255652</v>
-      </c>
-      <c r="J40" s="18">
-        <v>273332</v>
-      </c>
-      <c r="K40" s="17">
-        <f>L40/$P$7</f>
+        <f>J40/$N$7</f>
         <v>79621.087513033694</v>
       </c>
-      <c r="L40" s="15">
-        <f>J40*$L$41/$J$41</f>
+      <c r="J40" s="15">
+        <f>H40*$J$41/$H$41</f>
         <v>273140.3795767246</v>
       </c>
-      <c r="M40" s="26">
+      <c r="K40" s="26">
         <f t="shared" si="0"/>
         <v>1.2047919789524975</v>
       </c>
-      <c r="N40" s="15"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L40" s="15"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="10">
-        <f>SUM(C37:C40)</f>
+        <v>630451</v>
+      </c>
+      <c r="D41" s="14">
+        <f>SUM(D37:D40)</f>
+        <v>877094.65176100004</v>
+      </c>
+      <c r="E41" s="10">
+        <f>SUM(E37:E40)</f>
         <v>630453</v>
       </c>
-      <c r="D41" s="11">
-        <f>SUM(D37:D40)</f>
-        <v>905631.19809399999</v>
-      </c>
-      <c r="E41" s="10">
-        <v>630451</v>
-      </c>
-      <c r="F41" s="14">
+      <c r="F41" s="11">
         <f>SUM(F37:F40)</f>
-        <v>877094.65176100004</v>
+        <v>877124.60685999994</v>
       </c>
       <c r="G41" s="10">
-        <f>SUM(G37:G40)</f>
+        <f>E41</f>
         <v>630453</v>
       </c>
       <c r="H41" s="11">
         <f>SUM(H37:H40)</f>
-        <v>877124.60685999994</v>
+        <v>968542</v>
       </c>
       <c r="I41" s="10">
         <f>C41</f>
-        <v>630453</v>
-      </c>
-      <c r="J41" s="11">
-        <f>SUM(J37:J40)</f>
-        <v>968542</v>
-      </c>
-      <c r="K41" s="10">
-        <f>E41</f>
         <v>630451</v>
       </c>
-      <c r="L41" s="14">
+      <c r="J41" s="14">
         <v>967863</v>
       </c>
-      <c r="M41" s="27">
+      <c r="K41" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N41" s="15"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L41" s="15"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -3555,21 +3422,22 @@
         <v>12</v>
       </c>
       <c r="C42" s="6">
-        <v>36026</v>
-      </c>
-      <c r="D42" s="7">
+        <v>37665</v>
+      </c>
+      <c r="D42" s="15">
         <f>0*C42</f>
         <v>0</v>
       </c>
       <c r="E42" s="6">
-        <v>37665</v>
-      </c>
-      <c r="F42" s="15">
+        <v>38072</v>
+      </c>
+      <c r="F42" s="7">
         <f>0*E42</f>
         <v>0</v>
       </c>
       <c r="G42" s="6">
-        <v>38072</v>
+        <f>G46-SUM(G43:G45)</f>
+        <v>30350.092497222708</v>
       </c>
       <c r="H42" s="7">
         <f>0*G42</f>
@@ -3577,215 +3445,178 @@
       </c>
       <c r="I42" s="6">
         <f>I46-SUM(I43:I45)</f>
-        <v>30350.092497222708</v>
-      </c>
-      <c r="J42" s="7">
-        <f>0*I42</f>
+        <v>29838.601704968867</v>
+      </c>
+      <c r="J42" s="15">
+        <f>H42*$J$46/$H$46</f>
         <v>0</v>
       </c>
-      <c r="K42" s="6">
-        <f>K46-SUM(K43:K45)</f>
-        <v>29838.601704968867</v>
-      </c>
-      <c r="L42" s="15">
-        <f>J42*$L$46/$J$46</f>
-        <v>0</v>
-      </c>
-      <c r="M42" s="25">
-        <f>K42/E42</f>
+      <c r="K42" s="25">
+        <f>I42/C42</f>
         <v>0.79221032005758307</v>
       </c>
-      <c r="N42" s="15"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L42" s="15"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="6">
-        <v>53166</v>
-      </c>
-      <c r="D43" s="7">
+        <v>54266</v>
+      </c>
+      <c r="D43" s="15">
         <f>1*C43</f>
-        <v>53166</v>
+        <v>54266</v>
       </c>
       <c r="E43" s="6">
-        <v>54266</v>
-      </c>
-      <c r="F43" s="15">
+        <v>54057</v>
+      </c>
+      <c r="F43" s="7">
         <f>1*E43</f>
-        <v>54266</v>
+        <v>54057</v>
       </c>
       <c r="G43" s="6">
-        <v>54057</v>
+        <f>H43/1</f>
+        <v>55914</v>
       </c>
       <c r="H43" s="7">
-        <f>1*G43</f>
-        <v>54057</v>
+        <v>55914</v>
       </c>
       <c r="I43" s="6">
         <f>J43/1</f>
-        <v>55914</v>
-      </c>
-      <c r="J43" s="7">
-        <v>55914</v>
-      </c>
-      <c r="K43" s="6">
-        <f>L43/1</f>
         <v>56158.43615295249</v>
       </c>
-      <c r="L43" s="15">
-        <f>J43*$L$46/$J$46</f>
+      <c r="J43" s="15">
+        <f>H43*$J$46/$H$46</f>
         <v>56158.43615295249</v>
       </c>
-      <c r="M43" s="25">
+      <c r="K43" s="25">
         <f t="shared" si="0"/>
         <v>1.0348733305007278</v>
       </c>
-      <c r="N43" s="15"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L43" s="15"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="6">
-        <v>43919</v>
-      </c>
-      <c r="D44" s="7">
+        <v>41863</v>
+      </c>
+      <c r="D44" s="15">
         <f>2*C44</f>
-        <v>87838</v>
+        <v>83726</v>
       </c>
       <c r="E44" s="6">
-        <v>41863</v>
-      </c>
-      <c r="F44" s="15">
+        <v>42100</v>
+      </c>
+      <c r="F44" s="7">
         <f>2*E44</f>
-        <v>83726</v>
+        <v>84200</v>
       </c>
       <c r="G44" s="6">
-        <v>42100</v>
+        <f>H44/2</f>
+        <v>45984</v>
       </c>
       <c r="H44" s="7">
-        <f>2*G44</f>
-        <v>84200</v>
+        <v>91968</v>
       </c>
       <c r="I44" s="6">
         <f>J44/2</f>
-        <v>45984</v>
-      </c>
-      <c r="J44" s="7">
-        <v>91968</v>
-      </c>
-      <c r="K44" s="6">
-        <f>L44/2</f>
         <v>46185.025719093021</v>
       </c>
-      <c r="L44" s="15">
-        <f>J44*$L$46/$J$46</f>
+      <c r="J44" s="15">
+        <f>H44*$J$46/$H$46</f>
         <v>92370.051438186041</v>
       </c>
-      <c r="M44" s="25">
+      <c r="K44" s="25">
         <f t="shared" si="0"/>
         <v>1.1032421402931711</v>
       </c>
-      <c r="N44" s="15"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L44" s="15"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="12"/>
       <c r="B45" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="17">
-        <v>14241</v>
-      </c>
-      <c r="D45" s="18">
-        <f>C45*$P$7</f>
-        <v>48853.793223000001</v>
+        <v>13558</v>
+      </c>
+      <c r="D45" s="13">
+        <f>C45*$N$7</f>
+        <v>46510.759674000001</v>
       </c>
       <c r="E45" s="17">
-        <v>13558</v>
-      </c>
-      <c r="F45" s="13">
-        <f>E45*$P$7</f>
-        <v>46510.759674000001</v>
+        <v>13123</v>
+      </c>
+      <c r="F45" s="18">
+        <f>E45*$N$7</f>
+        <v>45018.490869000001</v>
       </c>
       <c r="G45" s="17">
-        <v>13123</v>
+        <f>H45/$N$7</f>
+        <v>15103.907502777291</v>
       </c>
       <c r="H45" s="18">
-        <f>G45*$P$7</f>
-        <v>45018.490869000001</v>
+        <v>51814</v>
       </c>
       <c r="I45" s="17">
-        <f>J45/$P$7</f>
-        <v>15103.907502777291</v>
-      </c>
-      <c r="J45" s="18">
-        <v>51814</v>
-      </c>
-      <c r="K45" s="17">
-        <f>L45/$P$7</f>
+        <f>J45/$N$7</f>
         <v>15169.936422985629</v>
       </c>
-      <c r="L45" s="15">
-        <f>J45*$L$46/$J$46</f>
+      <c r="J45" s="15">
+        <f>H45*$J$46/$H$46</f>
         <v>52040.512408861468</v>
       </c>
-      <c r="M45" s="26">
+      <c r="K45" s="26">
         <f t="shared" si="0"/>
         <v>1.1188919031557478</v>
       </c>
-      <c r="N45" s="15"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L45" s="15"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="10">
-        <f>SUM(C42:C45)</f>
         <v>147352</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="14">
         <f>SUM(D42:D45)</f>
-        <v>189857.79322300002</v>
+        <v>184502.759674</v>
       </c>
       <c r="E46" s="10">
+        <f>SUM(E42:E45)</f>
         <v>147352</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="11">
         <f>SUM(F42:F45)</f>
-        <v>184502.759674</v>
+        <v>183275.490869</v>
       </c>
       <c r="G46" s="10">
-        <f>SUM(G42:G45)</f>
+        <f>E46</f>
         <v>147352</v>
       </c>
       <c r="H46" s="11">
         <f>SUM(H42:H45)</f>
-        <v>183275.490869</v>
+        <v>199696</v>
       </c>
       <c r="I46" s="10">
         <f>C46</f>
         <v>147352</v>
       </c>
-      <c r="J46" s="11">
-        <f>SUM(J42:J45)</f>
-        <v>199696</v>
-      </c>
-      <c r="K46" s="10">
-        <f>E46</f>
-        <v>147352</v>
-      </c>
-      <c r="L46" s="14">
+      <c r="J46" s="14">
         <v>200569</v>
       </c>
-      <c r="M46" s="27">
+      <c r="K46" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N46" s="15"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L46" s="15"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -3793,21 +3624,22 @@
         <v>12</v>
       </c>
       <c r="C47" s="6">
-        <v>48946</v>
-      </c>
-      <c r="D47" s="7">
+        <v>51489</v>
+      </c>
+      <c r="D47" s="15">
         <f>0*C47</f>
         <v>0</v>
       </c>
       <c r="E47" s="6">
-        <v>51489</v>
-      </c>
-      <c r="F47" s="15">
+        <v>50709</v>
+      </c>
+      <c r="F47" s="7">
         <f>0*E47</f>
         <v>0</v>
       </c>
       <c r="G47" s="6">
-        <v>50709</v>
+        <f>G51-SUM(G48:G50)</f>
+        <v>41559.688059885084</v>
       </c>
       <c r="H47" s="7">
         <f>0*G47</f>
@@ -3815,215 +3647,178 @@
       </c>
       <c r="I47" s="6">
         <f>I51-SUM(I48:I50)</f>
-        <v>41559.688059885084</v>
-      </c>
-      <c r="J47" s="7">
-        <f>0*I47</f>
+        <v>42038.659486928314</v>
+      </c>
+      <c r="J47" s="15">
+        <f>H47*$J$51/$H$51</f>
         <v>0</v>
       </c>
-      <c r="K47" s="6">
-        <f>K51-SUM(K48:K50)</f>
-        <v>42038.659486928314</v>
-      </c>
-      <c r="L47" s="15">
-        <f>J47*$L$51/$J$51</f>
-        <v>0</v>
-      </c>
-      <c r="M47" s="25">
-        <f>K47/E47</f>
+      <c r="K47" s="25">
+        <f>I47/C47</f>
         <v>0.81645903954103427</v>
       </c>
-      <c r="N47" s="15"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L47" s="15"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="6">
-        <v>68952</v>
-      </c>
-      <c r="D48" s="7">
+        <v>69025</v>
+      </c>
+      <c r="D48" s="15">
         <f>1*C48</f>
-        <v>68952</v>
+        <v>69025</v>
       </c>
       <c r="E48" s="6">
-        <v>69025</v>
-      </c>
-      <c r="F48" s="15">
+        <v>69831</v>
+      </c>
+      <c r="F48" s="7">
         <f>1*E48</f>
-        <v>69025</v>
+        <v>69831</v>
       </c>
       <c r="G48" s="6">
-        <v>69831</v>
+        <f>H48/1</f>
+        <v>72470</v>
       </c>
       <c r="H48" s="7">
-        <f>1*G48</f>
-        <v>69831</v>
+        <v>72470</v>
       </c>
       <c r="I48" s="6">
         <f>J48/1</f>
-        <v>72470</v>
-      </c>
-      <c r="J48" s="7">
-        <v>72470</v>
-      </c>
-      <c r="K48" s="6">
-        <f>L48/1</f>
         <v>72236.252835710213</v>
       </c>
-      <c r="L48" s="15">
-        <f>J48*$L$51/$J$51</f>
+      <c r="J48" s="15">
+        <f>H48*$J$51/$H$51</f>
         <v>72236.252835710213</v>
       </c>
-      <c r="M48" s="25">
+      <c r="K48" s="25">
         <f t="shared" si="0"/>
         <v>1.0465230399958017</v>
       </c>
-      <c r="N48" s="15"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L48" s="15"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="6">
-        <v>55908</v>
-      </c>
-      <c r="D49" s="7">
+        <v>53747</v>
+      </c>
+      <c r="D49" s="15">
         <f>2*C49</f>
-        <v>111816</v>
+        <v>107494</v>
       </c>
       <c r="E49" s="6">
-        <v>53747</v>
-      </c>
-      <c r="F49" s="15">
+        <v>54083</v>
+      </c>
+      <c r="F49" s="7">
         <f>2*E49</f>
-        <v>107494</v>
+        <v>108166</v>
       </c>
       <c r="G49" s="6">
-        <v>54083</v>
+        <f>H49/2</f>
+        <v>57648.5</v>
       </c>
       <c r="H49" s="7">
-        <f>2*G49</f>
-        <v>108166</v>
+        <v>115297</v>
       </c>
       <c r="I49" s="6">
         <f>J49/2</f>
-        <v>57648.5</v>
-      </c>
-      <c r="J49" s="7">
-        <v>115297</v>
-      </c>
-      <c r="K49" s="6">
-        <f>L49/2</f>
         <v>57462.558598032847</v>
       </c>
-      <c r="L49" s="15">
-        <f>J49*$L$51/$J$51</f>
+      <c r="J49" s="15">
+        <f>H49*$J$51/$H$51</f>
         <v>114925.11719606569</v>
       </c>
-      <c r="M49" s="25">
+      <c r="K49" s="25">
         <f t="shared" si="0"/>
         <v>1.0691305300394971</v>
       </c>
-      <c r="N49" s="15"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L49" s="15"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="12"/>
       <c r="B50" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="17">
-        <v>16252</v>
-      </c>
-      <c r="D50" s="18">
-        <f>C50*$P$7</f>
-        <v>55752.534756000001</v>
+        <v>15797</v>
+      </c>
+      <c r="D50" s="13">
+        <f>C50*$N$7</f>
+        <v>54191.655890999995</v>
       </c>
       <c r="E50" s="17">
-        <v>15797</v>
-      </c>
-      <c r="F50" s="13">
-        <f>E50*$P$7</f>
-        <v>54191.655890999995</v>
+        <v>15435</v>
+      </c>
+      <c r="F50" s="18">
+        <f>E50*$N$7</f>
+        <v>52949.813804999998</v>
       </c>
       <c r="G50" s="17">
-        <v>15435</v>
+        <f>H50/$N$7</f>
+        <v>18379.811940114905</v>
       </c>
       <c r="H50" s="18">
-        <f>G50*$P$7</f>
-        <v>52949.813804999998</v>
+        <v>63052</v>
       </c>
       <c r="I50" s="17">
-        <f>J50/$P$7</f>
-        <v>18379.811940114905</v>
-      </c>
-      <c r="J50" s="18">
-        <v>63052</v>
-      </c>
-      <c r="K50" s="17">
-        <f>L50/$P$7</f>
+        <f>J50/$N$7</f>
         <v>18320.529079328629</v>
       </c>
-      <c r="L50" s="15">
-        <f>J50*$L$51/$J$51</f>
+      <c r="J50" s="15">
+        <f>H50*$J$51/$H$51</f>
         <v>62848.629968224101</v>
       </c>
-      <c r="M50" s="26">
+      <c r="K50" s="26">
         <f t="shared" si="0"/>
         <v>1.1597473621148717</v>
       </c>
-      <c r="N50" s="15"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L50" s="15"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="10">
-        <f>SUM(C47:C50)</f>
         <v>190058</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="14">
         <f>SUM(D47:D50)</f>
-        <v>236520.53475600001</v>
+        <v>230710.655891</v>
       </c>
       <c r="E51" s="10">
+        <f>SUM(E47:E50)</f>
         <v>190058</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="11">
         <f>SUM(F47:F50)</f>
-        <v>230710.655891</v>
+        <v>230946.81380499998</v>
       </c>
       <c r="G51" s="10">
-        <f>SUM(G47:G50)</f>
+        <f>E51</f>
         <v>190058</v>
       </c>
       <c r="H51" s="11">
         <f>SUM(H47:H50)</f>
-        <v>230946.81380499998</v>
+        <v>250819</v>
       </c>
       <c r="I51" s="10">
         <f>C51</f>
         <v>190058</v>
       </c>
-      <c r="J51" s="11">
-        <f>SUM(J47:J50)</f>
-        <v>250819</v>
-      </c>
-      <c r="K51" s="10">
-        <f>E51</f>
-        <v>190058</v>
-      </c>
-      <c r="L51" s="14">
+      <c r="J51" s="14">
         <v>250010</v>
       </c>
-      <c r="M51" s="27">
+      <c r="K51" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N51" s="15"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L51" s="15"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>19</v>
       </c>
@@ -4031,259 +3826,218 @@
         <v>12</v>
       </c>
       <c r="C52" s="6">
-        <f t="shared" ref="C52:D54" si="1">C7+C12+C17+C22+C27+C32+C37+C42+C47</f>
-        <v>560388</v>
-      </c>
-      <c r="D52" s="7">
+        <f t="shared" ref="C52:D52" si="1">C7+C12+C17+C22+C27+C32+C37+C42+C47</f>
+        <v>614314</v>
+      </c>
+      <c r="D52" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E52" s="6">
         <f t="shared" ref="E52:F52" si="2">E7+E12+E17+E22+E27+E32+E37+E42+E47</f>
-        <v>614314</v>
-      </c>
-      <c r="F52" s="15">
+        <v>616247</v>
+      </c>
+      <c r="F52" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G52" s="6">
-        <f t="shared" ref="G52:H52" si="3">G7+G12+G17+G22+G27+G32+G37+G42+G47</f>
-        <v>616247</v>
+        <f>G56-SUM(G53:G55)</f>
+        <v>438331.87515300233</v>
       </c>
       <c r="H52" s="7">
+        <f t="shared" ref="H52:I52" si="3">H7+H12+H17+H22+H27+H32+H37+H42+H47</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="23">
         <f t="shared" si="3"/>
+        <v>437806.66760893882</v>
+      </c>
+      <c r="J52" s="15">
+        <f t="shared" ref="J52" si="4">J7+J12+J17+J22+J27+J32+J37+J42+J47</f>
         <v>0</v>
       </c>
-      <c r="I52" s="6">
-        <f>I56-SUM(I53:I55)</f>
-        <v>438331.87515300233</v>
-      </c>
-      <c r="J52" s="7">
-        <f t="shared" ref="J52:K52" si="4">J7+J12+J17+J22+J27+J32+J37+J42+J47</f>
-        <v>0</v>
-      </c>
-      <c r="K52" s="23">
-        <f t="shared" si="4"/>
-        <v>437806.66760893882</v>
-      </c>
-      <c r="L52" s="15">
-        <f t="shared" ref="L52" si="5">L7+L12+L17+L22+L27+L32+L37+L42+L47</f>
-        <v>0</v>
-      </c>
-      <c r="M52" s="28">
-        <f>K52/E52</f>
+      <c r="K52" s="28">
+        <f>I52/C52</f>
         <v>0.71267571243523475</v>
       </c>
-      <c r="N52" s="15"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L52" s="15"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C53" s="6">
-        <f t="shared" si="1"/>
-        <v>1005220</v>
-      </c>
-      <c r="D53" s="7">
-        <f t="shared" si="1"/>
-        <v>1005220</v>
+        <f t="shared" ref="C53:D53" si="5">C8+C13+C18+C23+C28+C33+C38+C43+C48</f>
+        <v>1015350</v>
+      </c>
+      <c r="D53" s="15">
+        <f t="shared" si="5"/>
+        <v>1015350</v>
       </c>
       <c r="E53" s="6">
         <f t="shared" ref="E53:F53" si="6">E8+E13+E18+E23+E28+E33+E38+E43+E48</f>
-        <v>1015350</v>
-      </c>
-      <c r="F53" s="15">
+        <v>1014108</v>
+      </c>
+      <c r="F53" s="7">
         <f t="shared" si="6"/>
-        <v>1015350</v>
+        <v>1014108</v>
       </c>
       <c r="G53" s="6">
-        <f t="shared" ref="G53:H53" si="7">G8+G13+G18+G23+G28+G33+G38+G43+G48</f>
-        <v>1014108</v>
+        <f>H53/1</f>
+        <v>1060263</v>
       </c>
       <c r="H53" s="7">
+        <f t="shared" ref="H53:I53" si="7">H8+H13+H18+H23+H28+H33+H38+H43+H48</f>
+        <v>1060263</v>
+      </c>
+      <c r="I53" s="6">
         <f t="shared" si="7"/>
-        <v>1014108</v>
-      </c>
-      <c r="I53" s="6">
-        <f>J53/1</f>
-        <v>1060263</v>
-      </c>
-      <c r="J53" s="7">
-        <f t="shared" ref="J53:K53" si="8">J8+J13+J18+J23+J28+J33+J38+J43+J48</f>
-        <v>1060263</v>
-      </c>
-      <c r="K53" s="6">
-        <f t="shared" si="8"/>
         <v>1060557.4732710901</v>
       </c>
-      <c r="L53" s="15">
-        <f t="shared" ref="L53" si="9">L8+L13+L18+L23+L28+L33+L38+L43+L48</f>
+      <c r="J53" s="15">
+        <f t="shared" ref="J53" si="8">J8+J13+J18+J23+J28+J33+J38+J43+J48</f>
         <v>1060557.4732710901</v>
       </c>
-      <c r="M53" s="25">
+      <c r="K53" s="25">
         <f t="shared" si="0"/>
         <v>1.0445240294195008</v>
       </c>
-      <c r="N53" s="15"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L53" s="15"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="6">
-        <f t="shared" si="1"/>
-        <v>869278</v>
-      </c>
-      <c r="D54" s="7">
-        <f t="shared" si="1"/>
-        <v>1738556</v>
+        <f t="shared" ref="C54:D54" si="9">C9+C14+C19+C24+C29+C34+C39+C44+C49</f>
+        <v>825242</v>
+      </c>
+      <c r="D54" s="15">
+        <f t="shared" si="9"/>
+        <v>1650484</v>
       </c>
       <c r="E54" s="6">
         <f t="shared" ref="E54:F54" si="10">E9+E14+E19+E24+E29+E34+E39+E44+E49</f>
-        <v>825242</v>
-      </c>
-      <c r="F54" s="15">
+        <v>824603</v>
+      </c>
+      <c r="F54" s="7">
         <f t="shared" si="10"/>
-        <v>1650484</v>
+        <v>1649206</v>
       </c>
       <c r="G54" s="6">
-        <f t="shared" ref="G54:H54" si="11">G9+G14+G19+G24+G29+G34+G39+G44+G49</f>
-        <v>824603</v>
+        <f>H54/2</f>
+        <v>902485</v>
       </c>
       <c r="H54" s="7">
+        <f t="shared" ref="H54:I55" si="11">H9+H14+H19+H24+H29+H34+H39+H44+H49</f>
+        <v>1804970</v>
+      </c>
+      <c r="I54" s="6">
         <f t="shared" si="11"/>
-        <v>1649206</v>
-      </c>
-      <c r="I54" s="6">
-        <f>J54/2</f>
-        <v>902485</v>
-      </c>
-      <c r="J54" s="7">
-        <f t="shared" ref="J54:K55" si="12">J9+J14+J19+J24+J29+J34+J39+J44+J49</f>
-        <v>1804970</v>
-      </c>
-      <c r="K54" s="6">
-        <f t="shared" si="12"/>
         <v>902692.52762680571</v>
       </c>
-      <c r="L54" s="15">
-        <f t="shared" ref="L54" si="13">L9+L14+L19+L24+L29+L34+L39+L44+L49</f>
+      <c r="J54" s="15">
+        <f t="shared" ref="J54" si="12">J9+J14+J19+J24+J29+J34+J39+J44+J49</f>
         <v>1805385.0552536114</v>
       </c>
-      <c r="M54" s="25">
+      <c r="K54" s="25">
         <f t="shared" si="0"/>
         <v>1.093851897536487</v>
       </c>
-      <c r="N54" s="15"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L54" s="15"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="12"/>
       <c r="B55" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="17">
         <f>C10+C15+C20+C25+C30+C35+C40+C45+C50</f>
-        <v>266098</v>
-      </c>
-      <c r="D55" s="18">
-        <f>C55*$P$7</f>
-        <v>912849.98729399999</v>
+        <v>246080</v>
+      </c>
+      <c r="D55" s="13">
+        <f>C55*$N$7</f>
+        <v>844178.17823999992</v>
       </c>
       <c r="E55" s="17">
         <f>E10+E15+E20+E25+E30+E35+E40+E45+E50</f>
-        <v>246080</v>
-      </c>
-      <c r="F55" s="13">
-        <f>E55*$P$7</f>
-        <v>844178.17823999992</v>
+        <v>246026</v>
+      </c>
+      <c r="F55" s="18">
+        <f>E55*$N$7</f>
+        <v>843992.93107799999</v>
       </c>
       <c r="G55" s="17">
-        <f>G10+G15+G20+G25+G30+G35+G40+G45+G50</f>
-        <v>246026</v>
+        <f>H55/$N$7</f>
+        <v>299904.12484699767</v>
       </c>
       <c r="H55" s="18">
-        <f>G55*$P$7</f>
-        <v>843992.93107799999</v>
+        <f t="shared" si="11"/>
+        <v>1028822</v>
       </c>
       <c r="I55" s="17">
-        <f>J55/$P$7</f>
-        <v>299904.12484699767</v>
-      </c>
-      <c r="J55" s="18">
-        <f t="shared" si="12"/>
-        <v>1028822</v>
-      </c>
-      <c r="K55" s="17">
-        <f>K10+K15+K20+K25+K30+K35+K40+K45+K50</f>
+        <f>I10+I15+I20+I25+I30+I35+I40+I45+I50</f>
         <v>299929.33149316552</v>
       </c>
-      <c r="L55" s="13">
-        <f>L10+L15+L20+L25+L30+L35+L40+L45+L50</f>
+      <c r="J55" s="13">
+        <f>J10+J15+J20+J25+J30+J35+J40+J45+J50</f>
         <v>1028908.4714752986</v>
       </c>
-      <c r="M55" s="26">
+      <c r="K55" s="26">
         <f t="shared" si="0"/>
         <v>1.2188285577583124</v>
       </c>
-      <c r="N55" s="15"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L55" s="15"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="10">
-        <f t="shared" ref="C56:H56" si="14">SUM(C52:C55)</f>
+        <f t="shared" ref="C56:F56" si="13">SUM(C52:C55)</f>
+        <v>2700986</v>
+      </c>
+      <c r="D56" s="14">
+        <f t="shared" si="13"/>
+        <v>3510012.1782399998</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="13"/>
         <v>2700984</v>
       </c>
-      <c r="D56" s="11">
-        <f t="shared" si="14"/>
-        <v>3656625.9872940001</v>
-      </c>
-      <c r="E56" s="10">
-        <f t="shared" si="14"/>
+      <c r="F56" s="11">
+        <f t="shared" si="13"/>
+        <v>3507306.931078</v>
+      </c>
+      <c r="G56" s="10">
+        <f>E56</f>
+        <v>2700984</v>
+      </c>
+      <c r="H56" s="11">
+        <f>SUM(H52:H55)</f>
+        <v>3894055</v>
+      </c>
+      <c r="I56" s="10">
+        <f>SUM(I52:I55)</f>
         <v>2700986</v>
       </c>
-      <c r="F56" s="14">
-        <f t="shared" si="14"/>
-        <v>3510012.1782399998</v>
-      </c>
-      <c r="G56" s="10">
-        <f t="shared" si="14"/>
-        <v>2700984</v>
-      </c>
-      <c r="H56" s="11">
-        <f t="shared" si="14"/>
-        <v>3507306.931078</v>
-      </c>
-      <c r="I56" s="10">
-        <f>C56</f>
-        <v>2700984</v>
-      </c>
-      <c r="J56" s="11">
-        <f>SUM(J52:J55)</f>
-        <v>3894055</v>
-      </c>
-      <c r="K56" s="10">
-        <f>SUM(K52:K55)</f>
-        <v>2700986</v>
-      </c>
-      <c r="L56" s="14">
+      <c r="J56" s="14">
         <v>3894851</v>
       </c>
-      <c r="M56" s="27">
+      <c r="K56" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N56" s="15"/>
+      <c r="L56" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
@@ -4292,11 +4046,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4832,5 +4586,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documentation for ACS and PUMS years (2013-2017)
</commit_message>
<xml_diff>
--- a/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
+++ b/utilities/taz-data-baseyears/2015/Workers/ACSPUMS_WorkerTotals_2013-2017_Comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrael\Documents\GitHub\travel-model-one\utilities\taz-data-baseyears\2015\Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1452D9C2-7DC5-41E0-B82B-2C70D46546DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748BA8FB-4FF2-425A-8F86-FB344196FBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,41 +35,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Shimon Israel</author>
-  </authors>
-  <commentList>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Shimon Israel:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-From this script:
-"GitHub\PUMS-Data\Analysis\ACS PUMS 2013-2017\Worker Research\ACS 2013-2017 PUMS HH and Person Worker Research.R"</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shimon Israel</author>
@@ -200,7 +165,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Shimon Israel</author>
@@ -235,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="62">
   <si>
     <t>Alameda</t>
   </si>
@@ -331,9 +296,6 @@
   </si>
   <si>
     <t>Average No. Workers in 3+-Worker HHs</t>
-  </si>
-  <si>
-    <t>ACS and PUMS Data, 2012-2016</t>
   </si>
   <si>
     <t>San Francisco Total</t>
@@ -389,9 +351,6 @@
   </si>
   <si>
     <t>hh_wrks_3_plus</t>
-  </si>
-  <si>
-    <t>ACS and PUMS Data 2013-2017, and ACS 2013-2017</t>
   </si>
   <si>
     <t>PUMS 2013-2017 Person Weights</t>
@@ -467,6 +426,12 @@
   </si>
   <si>
     <t xml:space="preserve">These are for comparison with Columns C+D and come from PUMS data, ESR==1,4, which are workers actively working the ACS reference week (not total workers, as sick/vacationing workers are omitted). Columns C/D and E/F closely match, which means B08202 is not total workers but rather commuters and skews the household worker distribution lower, including overrepresenting 0-worker households. </t>
+  </si>
+  <si>
+    <t>ACS and PUMS Data, 2013-2017</t>
+  </si>
+  <si>
+    <t>ACS and PUMS Data 2013-2017</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1145,7 @@
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1254,6 +1219,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1574,11 +1540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1601,7 +1567,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1615,12 +1581,12 @@
     <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="37"/>
       <c r="E6" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>17</v>
@@ -1631,10 +1597,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>30</v>
@@ -1666,12 +1632,8 @@
       <c r="F8" s="7">
         <v>827795</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="16">
-        <v>3.4305029999999999</v>
-      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1872,7 +1834,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1880,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1908,12 +1869,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1923,46 +1884,46 @@
     </row>
     <row r="4" spans="1:14" ht="319" x14ac:dyDescent="0.35">
       <c r="C4" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J4" s="34"/>
       <c r="K4" s="33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="39"/>
       <c r="G5" s="38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H5" s="39"/>
       <c r="I5" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J5" s="39"/>
       <c r="K5" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1973,31 +1934,31 @@
         <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="G6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="32" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -2978,7 +2939,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="10">
@@ -4070,16 +4031,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -4090,7 +4051,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>0.7243926284066956</v>
@@ -4104,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1">
         <v>0.71045461057797943</v>
@@ -4118,7 +4079,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1">
         <v>0.65234440973873298</v>
@@ -4132,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1">
         <v>0.61093155138835786</v>
@@ -4146,7 +4107,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1">
         <v>0.81432449606111224</v>
@@ -4160,7 +4121,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1">
         <v>0.79221032005758307</v>
@@ -4174,7 +4135,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>0.71025600208376349</v>
@@ -4188,7 +4149,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1">
         <v>0.81645903954103427</v>
@@ -4202,7 +4163,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1">
         <v>0.81952491588983412</v>
@@ -4216,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1">
         <v>1.0549854708758115</v>
@@ -4230,7 +4191,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1">
         <v>1.0162564381618149</v>
@@ -4244,7 +4205,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1">
         <v>1.0467479421237909</v>
@@ -4258,7 +4219,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1">
         <v>1.0636388531450143</v>
@@ -4272,7 +4233,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1">
         <v>1.0207878838846087</v>
@@ -4286,7 +4247,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1">
         <v>1.0348733305007278</v>
@@ -4300,7 +4261,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1">
         <v>1.0667906227589079</v>
@@ -4314,7 +4275,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1">
         <v>1.0465230399958017</v>
@@ -4328,7 +4289,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1">
         <v>1.0466453858424083</v>
@@ -4342,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1">
         <v>1.077399993791341</v>
@@ -4356,7 +4317,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1">
         <v>1.080655652908822</v>
@@ -4370,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1">
         <v>1.0807546811717326</v>
@@ -4384,7 +4345,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1">
         <v>1.1506869686500032</v>
@@ -4398,7 +4359,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1">
         <v>1.0761103527203895</v>
@@ -4412,7 +4373,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1">
         <v>1.1032421402931711</v>
@@ -4426,7 +4387,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1">
         <v>1.0848258755408788</v>
@@ -4440,7 +4401,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1">
         <v>1.0691305300394971</v>
@@ -4454,7 +4415,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1">
         <v>1.0649963701049894</v>
@@ -4468,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="1">
         <v>1.2175676189166291</v>
@@ -4482,7 +4443,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1">
         <v>1.2111886446550346</v>
@@ -4496,7 +4457,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="1">
         <v>1.2047919789524975</v>
@@ -4510,7 +4471,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1">
         <v>1.3420147906012951</v>
@@ -4524,7 +4485,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1">
         <v>1.1536676698765049</v>
@@ -4538,7 +4499,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1">
         <v>1.1188919031557478</v>
@@ -4552,7 +4513,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1">
         <v>1.2652338137782535</v>
@@ -4566,7 +4527,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1">
         <v>1.1597473621148717</v>
@@ -4580,7 +4541,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" s="1">
         <v>1.1826070606325927</v>

</xml_diff>